<commit_message>
selesai penulisan skripsi 1
</commit_message>
<xml_diff>
--- a/Data Master & Uji/Data Perhitungan.xlsx
+++ b/Data Master & Uji/Data Perhitungan.xlsx
@@ -763,7 +763,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +823,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -904,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,6 +1044,44 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -22641,8 +22692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B293" sqref="B293:I330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26465,44 +26516,44 @@
       </c>
     </row>
     <row r="150" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B150" s="17">
+      <c r="B150" s="56">
         <v>1.2</v>
       </c>
-      <c r="C150" s="23" t="s">
+      <c r="C150" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="D150" s="24"/>
-      <c r="E150" s="24">
+      <c r="D150" s="58"/>
+      <c r="E150" s="58">
         <v>93</v>
       </c>
-      <c r="F150" s="24">
+      <c r="F150" s="58">
         <v>17</v>
       </c>
-      <c r="G150" s="24">
+      <c r="G150" s="58">
         <f>(E150-F150)</f>
         <v>76</v>
       </c>
-      <c r="H150" s="24">
+      <c r="H150" s="58">
         <f>((-F150/E150)*IMLOG2(F150/E150)+(-G150/E150)*IMLOG2(G150/E150))</f>
         <v>0.68615494742020033</v>
       </c>
-      <c r="I150" s="24"/>
+      <c r="I150" s="58"/>
       <c r="J150" s="26"/>
       <c r="K150" s="55" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="151" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B151" s="19"/>
-      <c r="C151" s="19" t="s">
+      <c r="B151" s="59"/>
+      <c r="C151" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="D151" s="19"/>
-      <c r="E151" s="19"/>
-      <c r="F151" s="19"/>
-      <c r="G151" s="19"/>
-      <c r="H151" s="19"/>
-      <c r="I151" s="19">
+      <c r="D151" s="59"/>
+      <c r="E151" s="59"/>
+      <c r="F151" s="59"/>
+      <c r="G151" s="59"/>
+      <c r="H151" s="59"/>
+      <c r="I151" s="59">
         <f>(H150)-((E152/E150*H152)+(E153/E150*H153))</f>
         <v>6.7252936892603365E-4</v>
       </c>
@@ -26513,64 +26564,64 @@
       <c r="K151" s="55"/>
     </row>
     <row r="152" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B152" s="19"/>
-      <c r="C152" s="19"/>
-      <c r="D152" s="19" t="s">
+      <c r="B152" s="59"/>
+      <c r="C152" s="59"/>
+      <c r="D152" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="E152" s="19">
+      <c r="E152" s="59">
         <v>63</v>
       </c>
-      <c r="F152" s="19">
+      <c r="F152" s="59">
         <v>11</v>
       </c>
-      <c r="G152" s="19">
+      <c r="G152" s="59">
         <f>(E152-F152)</f>
         <v>52</v>
       </c>
-      <c r="H152" s="19">
+      <c r="H152" s="59">
         <f t="shared" ref="H152:H153" si="12">((-F152/E152)*IMLOG2(F152/E152)+(-G152/E152)*IMLOG2(G152/E152))</f>
         <v>0.66812733384361367</v>
       </c>
-      <c r="I152" s="19"/>
+      <c r="I152" s="59"/>
       <c r="J152" s="26"/>
       <c r="K152" s="55"/>
     </row>
     <row r="153" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B153" s="19"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19" t="s">
+      <c r="B153" s="59"/>
+      <c r="C153" s="59"/>
+      <c r="D153" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E153" s="19">
+      <c r="E153" s="59">
         <v>30</v>
       </c>
-      <c r="F153" s="19">
+      <c r="F153" s="59">
         <v>6</v>
       </c>
-      <c r="G153" s="19">
+      <c r="G153" s="59">
         <f>(E153-F153)</f>
         <v>24</v>
       </c>
-      <c r="H153" s="19">
+      <c r="H153" s="59">
         <f t="shared" si="12"/>
         <v>0.72192809488736165</v>
       </c>
-      <c r="I153" s="19"/>
+      <c r="I153" s="59"/>
       <c r="J153" s="26"/>
       <c r="K153" s="55"/>
     </row>
     <row r="154" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B154" s="39"/>
-      <c r="C154" s="39" t="s">
+      <c r="B154" s="60"/>
+      <c r="C154" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="D154" s="39"/>
-      <c r="E154" s="39"/>
-      <c r="F154" s="39"/>
-      <c r="G154" s="39"/>
-      <c r="H154" s="39"/>
-      <c r="I154" s="39">
+      <c r="D154" s="60"/>
+      <c r="E154" s="60"/>
+      <c r="F154" s="60"/>
+      <c r="G154" s="60"/>
+      <c r="H154" s="60"/>
+      <c r="I154" s="60">
         <f>(H150)-((E155/E150*H155)+(E156/E150*H156)+(E157/E150*H157)+(E158/E150*H158))</f>
         <v>7.2026536350274672E-2</v>
       </c>
@@ -26581,118 +26632,118 @@
       <c r="K154" s="55"/>
     </row>
     <row r="155" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B155" s="39"/>
-      <c r="C155" s="39"/>
-      <c r="D155" s="40" t="s">
+      <c r="B155" s="60"/>
+      <c r="C155" s="60"/>
+      <c r="D155" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="E155" s="39">
+      <c r="E155" s="60">
         <v>21</v>
       </c>
-      <c r="F155" s="39">
+      <c r="F155" s="60">
         <v>3</v>
       </c>
-      <c r="G155" s="39">
+      <c r="G155" s="60">
         <f t="shared" ref="G155:G157" si="13">E155-F155</f>
         <v>18</v>
       </c>
-      <c r="H155" s="39">
+      <c r="H155" s="60">
         <f t="shared" ref="H155:H157" si="14">((-F155/E155)*IMLOG2(F155/E155)+(-G155/E155)*IMLOG2(G155/E155))</f>
         <v>0.59167277858232681</v>
       </c>
-      <c r="I155" s="39"/>
+      <c r="I155" s="60"/>
       <c r="J155" s="42" t="s">
         <v>26</v>
       </c>
       <c r="K155" s="55"/>
     </row>
     <row r="156" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B156" s="39"/>
-      <c r="C156" s="39"/>
-      <c r="D156" s="40" t="s">
+      <c r="B156" s="60"/>
+      <c r="C156" s="60"/>
+      <c r="D156" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="E156" s="39">
+      <c r="E156" s="60">
         <v>48</v>
       </c>
-      <c r="F156" s="39">
+      <c r="F156" s="60">
         <v>6</v>
       </c>
-      <c r="G156" s="39">
+      <c r="G156" s="60">
         <f t="shared" si="13"/>
         <v>42</v>
       </c>
-      <c r="H156" s="39">
+      <c r="H156" s="60">
         <f t="shared" si="14"/>
         <v>0.54356444319959651</v>
       </c>
-      <c r="I156" s="39"/>
+      <c r="I156" s="60"/>
       <c r="J156" s="42" t="s">
         <v>229</v>
       </c>
       <c r="K156" s="55"/>
     </row>
     <row r="157" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B157" s="39"/>
-      <c r="C157" s="39"/>
-      <c r="D157" s="40" t="s">
+      <c r="B157" s="60"/>
+      <c r="C157" s="60"/>
+      <c r="D157" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="E157" s="39">
+      <c r="E157" s="60">
         <v>22</v>
       </c>
-      <c r="F157" s="39">
+      <c r="F157" s="60">
         <v>6</v>
       </c>
-      <c r="G157" s="39">
+      <c r="G157" s="60">
         <f t="shared" si="13"/>
         <v>16</v>
       </c>
-      <c r="H157" s="39">
+      <c r="H157" s="60">
         <f t="shared" si="14"/>
         <v>0.84535093662243588</v>
       </c>
-      <c r="I157" s="39"/>
+      <c r="I157" s="60"/>
       <c r="J157" s="42" t="s">
         <v>229</v>
       </c>
       <c r="K157" s="55"/>
     </row>
     <row r="158" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B158" s="39"/>
-      <c r="C158" s="39"/>
-      <c r="D158" s="39" t="s">
+      <c r="B158" s="60"/>
+      <c r="C158" s="60"/>
+      <c r="D158" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="E158" s="39">
+      <c r="E158" s="60">
         <v>2</v>
       </c>
-      <c r="F158" s="39">
+      <c r="F158" s="60">
         <v>2</v>
       </c>
-      <c r="G158" s="39">
-        <v>0</v>
-      </c>
-      <c r="H158" s="41">
-        <v>0</v>
-      </c>
-      <c r="I158" s="39"/>
+      <c r="G158" s="60">
+        <v>0</v>
+      </c>
+      <c r="H158" s="62">
+        <v>0</v>
+      </c>
+      <c r="I158" s="60"/>
       <c r="J158" s="42" t="s">
         <v>45</v>
       </c>
       <c r="K158" s="55"/>
     </row>
     <row r="159" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B159" s="19"/>
-      <c r="C159" s="19" t="s">
+      <c r="B159" s="59"/>
+      <c r="C159" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="D159" s="19"/>
-      <c r="E159" s="19"/>
-      <c r="F159" s="19"/>
-      <c r="G159" s="19"/>
-      <c r="H159" s="19"/>
-      <c r="I159" s="19">
+      <c r="D159" s="59"/>
+      <c r="E159" s="59"/>
+      <c r="F159" s="59"/>
+      <c r="G159" s="59"/>
+      <c r="H159" s="59"/>
+      <c r="I159" s="59">
         <f>(H150)-((E160/E150*H160)+(E161/E150*H161)+(E162/E150*H162))</f>
         <v>3.9566759442719257E-2</v>
       </c>
@@ -26703,87 +26754,87 @@
       <c r="K159" s="55"/>
     </row>
     <row r="160" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B160" s="19"/>
-      <c r="C160" s="19"/>
-      <c r="D160" s="19" t="s">
+      <c r="B160" s="59"/>
+      <c r="C160" s="59"/>
+      <c r="D160" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E160" s="19">
+      <c r="E160" s="59">
         <v>48</v>
       </c>
-      <c r="F160" s="19">
+      <c r="F160" s="59">
         <v>11</v>
       </c>
-      <c r="G160" s="19">
+      <c r="G160" s="59">
         <f>E160-F160</f>
         <v>37</v>
       </c>
-      <c r="H160" s="19">
+      <c r="H160" s="59">
         <f t="shared" ref="H160:H161" si="16">((-F160/E160)*IMLOG2(F160/E160)+(-G160/E160)*IMLOG2(G160/E160))</f>
         <v>0.77655578544446002</v>
       </c>
-      <c r="I160" s="19"/>
+      <c r="I160" s="59"/>
       <c r="J160" s="26"/>
       <c r="K160" s="55"/>
     </row>
     <row r="161" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B161" s="19"/>
-      <c r="C161" s="19"/>
-      <c r="D161" s="19" t="s">
+      <c r="B161" s="59"/>
+      <c r="C161" s="59"/>
+      <c r="D161" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="E161" s="19">
+      <c r="E161" s="59">
         <v>34</v>
       </c>
-      <c r="F161" s="19">
+      <c r="F161" s="59">
         <v>6</v>
       </c>
-      <c r="G161" s="19">
+      <c r="G161" s="59">
         <f t="shared" ref="G161:G162" si="17">E161-F161</f>
         <v>28</v>
       </c>
-      <c r="H161" s="19">
+      <c r="H161" s="59">
         <f t="shared" si="16"/>
         <v>0.6722948170756371</v>
       </c>
-      <c r="I161" s="19"/>
+      <c r="I161" s="59"/>
       <c r="J161" s="26"/>
       <c r="K161" s="55"/>
     </row>
     <row r="162" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B162" s="19"/>
-      <c r="C162" s="19"/>
-      <c r="D162" s="19" t="s">
+      <c r="B162" s="59"/>
+      <c r="C162" s="59"/>
+      <c r="D162" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="E162" s="19">
+      <c r="E162" s="59">
         <v>11</v>
       </c>
-      <c r="F162" s="19">
-        <v>0</v>
-      </c>
-      <c r="G162" s="19">
+      <c r="F162" s="59">
+        <v>0</v>
+      </c>
+      <c r="G162" s="59">
         <f t="shared" si="17"/>
         <v>11</v>
       </c>
-      <c r="H162" s="19">
-        <v>0</v>
-      </c>
-      <c r="I162" s="19"/>
+      <c r="H162" s="59">
+        <v>0</v>
+      </c>
+      <c r="I162" s="59"/>
       <c r="J162" s="26"/>
       <c r="K162" s="55"/>
     </row>
     <row r="163" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B163" s="19"/>
-      <c r="C163" s="19" t="s">
+      <c r="B163" s="59"/>
+      <c r="C163" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="D163" s="19"/>
-      <c r="E163" s="19"/>
-      <c r="F163" s="19"/>
-      <c r="G163" s="19"/>
-      <c r="H163" s="19"/>
-      <c r="I163" s="19">
+      <c r="D163" s="59"/>
+      <c r="E163" s="59"/>
+      <c r="F163" s="59"/>
+      <c r="G163" s="59"/>
+      <c r="H163" s="59"/>
+      <c r="I163" s="59">
         <f>(H150)-((E164/E150*H164)+(E165/E150*H165)+(E166/E150*H166)+(E167/E150*H167))</f>
         <v>1.2200694943823032E-2</v>
       </c>
@@ -26793,113 +26844,113 @@
       </c>
       <c r="K163" s="55"/>
     </row>
-    <row r="164" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B164" s="19"/>
-      <c r="C164" s="19"/>
-      <c r="D164" s="21" t="s">
+    <row r="164" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B164" s="59"/>
+      <c r="C164" s="59"/>
+      <c r="D164" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="E164" s="24">
+      <c r="E164" s="58">
         <v>15</v>
       </c>
-      <c r="F164" s="24">
+      <c r="F164" s="58">
         <v>2</v>
       </c>
-      <c r="G164" s="24">
+      <c r="G164" s="58">
         <f t="shared" ref="G164:G167" si="18">E164-F164</f>
         <v>13</v>
       </c>
-      <c r="H164" s="24">
+      <c r="H164" s="58">
         <f t="shared" ref="H164:H167" si="19">((-F164/E164)*IMLOG2(F164/E164)+(-G164/E164)*IMLOG2(G164/E164))</f>
         <v>0.56650950655290522</v>
       </c>
-      <c r="I164" s="19"/>
+      <c r="I164" s="59"/>
       <c r="J164" s="26"/>
       <c r="K164" s="55"/>
     </row>
     <row r="165" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B165" s="19"/>
-      <c r="C165" s="19"/>
-      <c r="D165" s="19" t="s">
+      <c r="B165" s="59"/>
+      <c r="C165" s="59"/>
+      <c r="D165" s="59" t="s">
         <v>159</v>
       </c>
-      <c r="E165" s="24">
+      <c r="E165" s="58">
         <v>8</v>
       </c>
-      <c r="F165" s="24">
+      <c r="F165" s="58">
         <v>2</v>
       </c>
-      <c r="G165" s="24">
+      <c r="G165" s="58">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="H165" s="24">
+      <c r="H165" s="58">
         <f t="shared" si="19"/>
         <v>0.81127812445913294</v>
       </c>
-      <c r="I165" s="19"/>
+      <c r="I165" s="59"/>
       <c r="J165" s="26"/>
       <c r="K165" s="55"/>
     </row>
-    <row r="166" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B166" s="19"/>
-      <c r="C166" s="19"/>
-      <c r="D166" s="21" t="s">
+    <row r="166" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B166" s="59"/>
+      <c r="C166" s="59"/>
+      <c r="D166" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="E166" s="24">
+      <c r="E166" s="58">
         <v>34</v>
       </c>
-      <c r="F166" s="24">
+      <c r="F166" s="58">
         <v>8</v>
       </c>
-      <c r="G166" s="24">
+      <c r="G166" s="58">
         <f t="shared" si="18"/>
         <v>26</v>
       </c>
-      <c r="H166" s="24">
+      <c r="H166" s="58">
         <f t="shared" si="19"/>
         <v>0.78712658620126885</v>
       </c>
-      <c r="I166" s="19"/>
+      <c r="I166" s="59"/>
       <c r="J166" s="26"/>
       <c r="K166" s="55"/>
     </row>
-    <row r="167" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B167" s="19"/>
-      <c r="C167" s="19"/>
-      <c r="D167" s="21" t="s">
+    <row r="167" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B167" s="59"/>
+      <c r="C167" s="59"/>
+      <c r="D167" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="E167" s="24">
+      <c r="E167" s="58">
         <v>36</v>
       </c>
-      <c r="F167" s="24">
+      <c r="F167" s="58">
         <v>5</v>
       </c>
-      <c r="G167" s="24">
+      <c r="G167" s="58">
         <f t="shared" si="18"/>
         <v>31</v>
       </c>
-      <c r="H167" s="24">
+      <c r="H167" s="58">
         <f t="shared" si="19"/>
         <v>0.58132149876370276</v>
       </c>
-      <c r="I167" s="19"/>
+      <c r="I167" s="59"/>
       <c r="J167" s="26"/>
       <c r="K167" s="55"/>
     </row>
     <row r="168" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B168" s="19"/>
-      <c r="C168" s="21" t="s">
+      <c r="B168" s="59"/>
+      <c r="C168" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="D168" s="19"/>
-      <c r="E168" s="19"/>
-      <c r="F168" s="19"/>
-      <c r="G168" s="19"/>
-      <c r="H168" s="19"/>
-      <c r="I168" s="19">
+      <c r="D168" s="59"/>
+      <c r="E168" s="59"/>
+      <c r="F168" s="59"/>
+      <c r="G168" s="59"/>
+      <c r="H168" s="59"/>
+      <c r="I168" s="59">
         <f>(H150)-((E169/E150*H169)+(E170/E150*H170)+(E171/E150*H171))</f>
         <v>1.832269768429251E-2</v>
       </c>
@@ -26910,88 +26961,88 @@
       <c r="K168" s="55"/>
     </row>
     <row r="169" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B169" s="19"/>
-      <c r="C169" s="19"/>
-      <c r="D169" s="21" t="s">
+      <c r="B169" s="59"/>
+      <c r="C169" s="59"/>
+      <c r="D169" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="E169" s="19">
+      <c r="E169" s="59">
         <v>8</v>
       </c>
-      <c r="F169" s="19">
+      <c r="F169" s="59">
         <v>3</v>
       </c>
-      <c r="G169" s="19">
+      <c r="G169" s="59">
         <f t="shared" ref="G169:G171" si="20">E169-F169</f>
         <v>5</v>
       </c>
-      <c r="H169" s="19">
+      <c r="H169" s="59">
         <f t="shared" ref="H169:H171" si="21">((-F169/E169)*IMLOG2(F169/E169)+(-G169/E169)*IMLOG2(G169/E169))</f>
         <v>0.95443400292496372</v>
       </c>
-      <c r="I169" s="19"/>
+      <c r="I169" s="59"/>
       <c r="J169" s="26"/>
       <c r="K169" s="55"/>
     </row>
     <row r="170" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B170" s="19"/>
-      <c r="C170" s="19"/>
-      <c r="D170" s="21" t="s">
+      <c r="B170" s="59"/>
+      <c r="C170" s="59"/>
+      <c r="D170" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="E170" s="19">
+      <c r="E170" s="59">
         <v>60</v>
       </c>
-      <c r="F170" s="19">
+      <c r="F170" s="59">
         <v>11</v>
       </c>
-      <c r="G170" s="19">
+      <c r="G170" s="59">
         <f t="shared" si="20"/>
         <v>49</v>
       </c>
-      <c r="H170" s="19">
+      <c r="H170" s="59">
         <f t="shared" si="21"/>
         <v>0.68731509283092684</v>
       </c>
-      <c r="I170" s="19"/>
+      <c r="I170" s="59"/>
       <c r="J170" s="26"/>
       <c r="K170" s="55"/>
     </row>
     <row r="171" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B171" s="19"/>
-      <c r="C171" s="19"/>
-      <c r="D171" s="21" t="s">
+      <c r="B171" s="59"/>
+      <c r="C171" s="59"/>
+      <c r="D171" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="E171" s="19">
+      <c r="E171" s="59">
         <v>25</v>
       </c>
-      <c r="F171" s="19">
+      <c r="F171" s="59">
         <v>3</v>
       </c>
-      <c r="G171" s="19">
+      <c r="G171" s="59">
         <f t="shared" si="20"/>
         <v>22</v>
       </c>
-      <c r="H171" s="19">
+      <c r="H171" s="59">
         <f t="shared" si="21"/>
         <v>0.52936086528736415</v>
       </c>
-      <c r="I171" s="19"/>
+      <c r="I171" s="59"/>
       <c r="J171" s="26"/>
       <c r="K171" s="55"/>
     </row>
     <row r="172" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B172" s="19"/>
-      <c r="C172" s="19" t="s">
+      <c r="B172" s="59"/>
+      <c r="C172" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="D172" s="19"/>
-      <c r="E172" s="19"/>
-      <c r="F172" s="19"/>
-      <c r="G172" s="19"/>
-      <c r="H172" s="19"/>
-      <c r="I172" s="19">
+      <c r="D172" s="59"/>
+      <c r="E172" s="59"/>
+      <c r="F172" s="59"/>
+      <c r="G172" s="59"/>
+      <c r="H172" s="59"/>
+      <c r="I172" s="59">
         <f>(H150)-((E173/E150*H173)+(E174/E150*H174)+(E175/E150*H175))</f>
         <v>6.1388395266426254E-3</v>
       </c>
@@ -27002,88 +27053,88 @@
       <c r="K172" s="55"/>
     </row>
     <row r="173" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B173" s="19"/>
-      <c r="C173" s="19"/>
-      <c r="D173" s="21" t="s">
+      <c r="B173" s="59"/>
+      <c r="C173" s="59"/>
+      <c r="D173" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="E173" s="19">
+      <c r="E173" s="59">
         <v>34</v>
       </c>
-      <c r="F173" s="19">
+      <c r="F173" s="59">
         <v>7</v>
       </c>
-      <c r="G173" s="19">
+      <c r="G173" s="59">
         <f t="shared" ref="G173:G175" si="22">E173-F173</f>
         <v>27</v>
       </c>
-      <c r="H173" s="19">
+      <c r="H173" s="59">
         <f>((-F173/E173)*IMLOG2(F173/E173)+(-G173/E173)*IMLOG2(G173/E173))</f>
         <v>0.73353792910866744</v>
       </c>
-      <c r="I173" s="19"/>
+      <c r="I173" s="59"/>
       <c r="J173" s="26"/>
       <c r="K173" s="55"/>
     </row>
     <row r="174" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B174" s="19"/>
-      <c r="C174" s="19"/>
-      <c r="D174" s="21" t="s">
+      <c r="B174" s="59"/>
+      <c r="C174" s="59"/>
+      <c r="D174" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="E174" s="19">
+      <c r="E174" s="59">
         <v>23</v>
       </c>
-      <c r="F174" s="19">
+      <c r="F174" s="59">
         <v>5</v>
       </c>
-      <c r="G174" s="19">
+      <c r="G174" s="59">
         <f t="shared" si="22"/>
         <v>18</v>
       </c>
-      <c r="H174" s="19">
+      <c r="H174" s="59">
         <f t="shared" ref="H174:H175" si="23">((-F174/E174)*IMLOG2(F174/E174)+(-G174/E174)*IMLOG2(G174/E174))</f>
         <v>0.75537541256142915</v>
       </c>
-      <c r="I174" s="19"/>
+      <c r="I174" s="59"/>
       <c r="J174" s="26"/>
       <c r="K174" s="55"/>
     </row>
     <row r="175" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B175" s="19"/>
-      <c r="C175" s="19"/>
-      <c r="D175" s="21" t="s">
+      <c r="B175" s="59"/>
+      <c r="C175" s="59"/>
+      <c r="D175" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="E175" s="19">
+      <c r="E175" s="59">
         <v>36</v>
       </c>
-      <c r="F175" s="19">
+      <c r="F175" s="59">
         <v>5</v>
       </c>
-      <c r="G175" s="19">
+      <c r="G175" s="59">
         <f t="shared" si="22"/>
         <v>31</v>
       </c>
-      <c r="H175" s="19">
+      <c r="H175" s="59">
         <f t="shared" si="23"/>
         <v>0.58132149876370276</v>
       </c>
-      <c r="I175" s="19"/>
+      <c r="I175" s="59"/>
       <c r="J175" s="26"/>
       <c r="K175" s="55"/>
     </row>
-    <row r="176" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B176" s="19"/>
-      <c r="C176" s="21" t="s">
+    <row r="176" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B176" s="59"/>
+      <c r="C176" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="D176" s="19"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="19"/>
-      <c r="G176" s="19"/>
-      <c r="H176" s="19"/>
-      <c r="I176" s="19">
+      <c r="D176" s="59"/>
+      <c r="E176" s="59"/>
+      <c r="F176" s="59"/>
+      <c r="G176" s="59"/>
+      <c r="H176" s="59"/>
+      <c r="I176" s="59">
         <f>(H150)-((E177/E150*H177)+(E178/E150*H178))</f>
         <v>3.9258206110145411E-3</v>
       </c>
@@ -27094,64 +27145,64 @@
       <c r="K176" s="55"/>
     </row>
     <row r="177" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
-      <c r="D177" s="21" t="s">
+      <c r="B177" s="59"/>
+      <c r="C177" s="59"/>
+      <c r="D177" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="E177" s="19">
+      <c r="E177" s="59">
         <v>42</v>
       </c>
-      <c r="F177" s="19">
+      <c r="F177" s="59">
         <v>9</v>
       </c>
-      <c r="G177" s="19">
+      <c r="G177" s="59">
         <f t="shared" ref="G177:G178" si="24">E177-F177</f>
         <v>33</v>
       </c>
-      <c r="H177" s="19">
+      <c r="H177" s="59">
         <f>((-F177/E177)*IMLOG2(F177/E177)+(-G177/E177)*IMLOG2(G177/E177))</f>
         <v>0.7495952572594804</v>
       </c>
-      <c r="I177" s="19"/>
+      <c r="I177" s="59"/>
       <c r="J177" s="26"/>
       <c r="K177" s="55"/>
     </row>
     <row r="178" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B178" s="19"/>
-      <c r="C178" s="19"/>
-      <c r="D178" s="21" t="s">
+      <c r="B178" s="59"/>
+      <c r="C178" s="59"/>
+      <c r="D178" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="E178" s="19">
+      <c r="E178" s="59">
         <v>51</v>
       </c>
-      <c r="F178" s="19">
+      <c r="F178" s="59">
         <v>8</v>
       </c>
-      <c r="G178" s="19">
+      <c r="G178" s="59">
         <f t="shared" si="24"/>
         <v>43</v>
       </c>
-      <c r="H178" s="19">
+      <c r="H178" s="59">
         <f t="shared" ref="H178" si="25">((-F178/E178)*IMLOG2(F178/E178)+(-G178/E178)*IMLOG2(G178/E178))</f>
         <v>0.62675113702659047</v>
       </c>
-      <c r="I178" s="19"/>
+      <c r="I178" s="59"/>
       <c r="J178" s="26"/>
       <c r="K178" s="55"/>
     </row>
-    <row r="179" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B179" s="19"/>
-      <c r="C179" s="21" t="s">
+    <row r="179" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B179" s="59"/>
+      <c r="C179" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="D179" s="19"/>
-      <c r="E179" s="19"/>
-      <c r="F179" s="19"/>
-      <c r="G179" s="19"/>
-      <c r="H179" s="19"/>
-      <c r="I179" s="19">
+      <c r="D179" s="59"/>
+      <c r="E179" s="59"/>
+      <c r="F179" s="59"/>
+      <c r="G179" s="59"/>
+      <c r="H179" s="59"/>
+      <c r="I179" s="59">
         <f>(H150)-((E180/E150*H180)+(E181/E150*H181)+(E182/E150*H182))</f>
         <v>5.5876376916906834E-3</v>
       </c>
@@ -27162,88 +27213,88 @@
       <c r="K179" s="55"/>
     </row>
     <row r="180" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B180" s="19"/>
-      <c r="C180" s="19"/>
-      <c r="D180" s="21" t="s">
+      <c r="B180" s="59"/>
+      <c r="C180" s="59"/>
+      <c r="D180" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="E180" s="19">
+      <c r="E180" s="59">
         <v>58</v>
       </c>
-      <c r="F180" s="19">
+      <c r="F180" s="59">
         <v>12</v>
       </c>
-      <c r="G180" s="19">
+      <c r="G180" s="59">
         <f t="shared" ref="G180:G182" si="26">E180-F180</f>
         <v>46</v>
       </c>
-      <c r="H180" s="19">
+      <c r="H180" s="59">
         <f t="shared" ref="H180:H182" si="27">((-F180/E180)*IMLOG2(F180/E180)+(-G180/E180)*IMLOG2(G180/E180))</f>
         <v>0.73550858155384047</v>
       </c>
-      <c r="I180" s="19"/>
+      <c r="I180" s="59"/>
       <c r="J180" s="26"/>
       <c r="K180" s="55"/>
     </row>
     <row r="181" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B181" s="19"/>
-      <c r="C181" s="19"/>
-      <c r="D181" s="21" t="s">
+      <c r="B181" s="59"/>
+      <c r="C181" s="59"/>
+      <c r="D181" s="63" t="s">
         <v>219</v>
       </c>
-      <c r="E181" s="19">
+      <c r="E181" s="59">
         <v>26</v>
       </c>
-      <c r="F181" s="19">
+      <c r="F181" s="59">
         <v>4</v>
       </c>
-      <c r="G181" s="19">
+      <c r="G181" s="59">
         <f t="shared" si="26"/>
         <v>22</v>
       </c>
-      <c r="H181" s="19">
+      <c r="H181" s="59">
         <f t="shared" si="27"/>
         <v>0.61938219467876343</v>
       </c>
-      <c r="I181" s="19"/>
+      <c r="I181" s="59"/>
       <c r="J181" s="26"/>
       <c r="K181" s="55"/>
     </row>
     <row r="182" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B182" s="19"/>
-      <c r="C182" s="19"/>
-      <c r="D182" s="21" t="s">
+      <c r="B182" s="59"/>
+      <c r="C182" s="59"/>
+      <c r="D182" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="E182" s="19">
+      <c r="E182" s="59">
         <v>9</v>
       </c>
-      <c r="F182" s="19">
+      <c r="F182" s="59">
         <v>1</v>
       </c>
-      <c r="G182" s="19">
+      <c r="G182" s="59">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="H182" s="19">
+      <c r="H182" s="59">
         <f t="shared" si="27"/>
         <v>0.50325833477564508</v>
       </c>
-      <c r="I182" s="19"/>
+      <c r="I182" s="59"/>
       <c r="J182" s="26"/>
       <c r="K182" s="55"/>
     </row>
-    <row r="183" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B183" s="19"/>
-      <c r="C183" s="21" t="s">
+    <row r="183" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B183" s="59"/>
+      <c r="C183" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="D183" s="19"/>
-      <c r="E183" s="19"/>
-      <c r="F183" s="19"/>
-      <c r="G183" s="19"/>
-      <c r="H183" s="19"/>
-      <c r="I183" s="19">
+      <c r="D183" s="59"/>
+      <c r="E183" s="59"/>
+      <c r="F183" s="59"/>
+      <c r="G183" s="59"/>
+      <c r="H183" s="59"/>
+      <c r="I183" s="59">
         <f>(H150)-((E184/E150*H184)+(E185/E150*H185)+(E186/E150*H186)+(E187/E150*H187))</f>
         <v>4.6476954891183753E-2</v>
       </c>
@@ -27254,112 +27305,112 @@
       <c r="K183" s="55"/>
     </row>
     <row r="184" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B184" s="19"/>
-      <c r="C184" s="19"/>
-      <c r="D184" s="21" t="s">
+      <c r="B184" s="59"/>
+      <c r="C184" s="59"/>
+      <c r="D184" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E184" s="19">
+      <c r="E184" s="59">
         <v>23</v>
       </c>
-      <c r="F184" s="19">
+      <c r="F184" s="59">
         <v>1</v>
       </c>
-      <c r="G184" s="19">
+      <c r="G184" s="59">
         <f t="shared" ref="G184:G187" si="28">E184-F184</f>
         <v>22</v>
       </c>
-      <c r="H184" s="19">
+      <c r="H184" s="59">
         <f t="shared" ref="H184:H187" si="29">((-F184/E184)*IMLOG2(F184/E184)+(-G184/E184)*IMLOG2(G184/E184))</f>
         <v>0.25801866866481538</v>
       </c>
-      <c r="I184" s="19"/>
+      <c r="I184" s="59"/>
       <c r="J184" s="26"/>
       <c r="K184" s="55"/>
     </row>
     <row r="185" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B185" s="19"/>
-      <c r="C185" s="19"/>
-      <c r="D185" s="21" t="s">
+      <c r="B185" s="59"/>
+      <c r="C185" s="59"/>
+      <c r="D185" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E185" s="19">
+      <c r="E185" s="59">
         <v>5</v>
       </c>
-      <c r="F185" s="19">
+      <c r="F185" s="59">
         <v>2</v>
       </c>
-      <c r="G185" s="19">
+      <c r="G185" s="59">
         <f t="shared" si="28"/>
         <v>3</v>
       </c>
-      <c r="H185" s="19">
+      <c r="H185" s="59">
         <f t="shared" si="29"/>
         <v>0.97095059445466747</v>
       </c>
-      <c r="I185" s="19"/>
+      <c r="I185" s="59"/>
       <c r="J185" s="26"/>
       <c r="K185" s="55"/>
     </row>
     <row r="186" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B186" s="19"/>
-      <c r="C186" s="19"/>
-      <c r="D186" s="21" t="s">
+      <c r="B186" s="59"/>
+      <c r="C186" s="59"/>
+      <c r="D186" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="E186" s="19">
+      <c r="E186" s="59">
         <v>12</v>
       </c>
-      <c r="F186" s="19">
+      <c r="F186" s="59">
         <v>2</v>
       </c>
-      <c r="G186" s="19">
+      <c r="G186" s="59">
         <f t="shared" si="28"/>
         <v>10</v>
       </c>
-      <c r="H186" s="19">
+      <c r="H186" s="59">
         <f t="shared" si="29"/>
         <v>0.650022421648355</v>
       </c>
-      <c r="I186" s="19"/>
+      <c r="I186" s="59"/>
       <c r="J186" s="26"/>
       <c r="K186" s="55"/>
     </row>
     <row r="187" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B187" s="19"/>
-      <c r="C187" s="19"/>
-      <c r="D187" s="21" t="s">
+      <c r="B187" s="59"/>
+      <c r="C187" s="59"/>
+      <c r="D187" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E187" s="19">
+      <c r="E187" s="59">
         <v>53</v>
       </c>
-      <c r="F187" s="19">
+      <c r="F187" s="59">
         <v>12</v>
       </c>
-      <c r="G187" s="19">
+      <c r="G187" s="59">
         <f t="shared" si="28"/>
         <v>41</v>
       </c>
-      <c r="H187" s="19">
+      <c r="H187" s="59">
         <f t="shared" si="29"/>
         <v>0.77170946969536214</v>
       </c>
-      <c r="I187" s="19"/>
+      <c r="I187" s="59"/>
       <c r="J187" s="26"/>
       <c r="K187" s="55"/>
     </row>
-    <row r="188" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B188" s="19"/>
-      <c r="C188" s="21" t="s">
+    <row r="188" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B188" s="59"/>
+      <c r="C188" s="63" t="s">
         <v>218</v>
       </c>
-      <c r="D188" s="19"/>
-      <c r="E188" s="19"/>
-      <c r="F188" s="19"/>
-      <c r="G188" s="19"/>
-      <c r="H188" s="19"/>
-      <c r="I188" s="19">
+      <c r="D188" s="59"/>
+      <c r="E188" s="59"/>
+      <c r="F188" s="59"/>
+      <c r="G188" s="59"/>
+      <c r="H188" s="59"/>
+      <c r="I188" s="59">
         <f>(H150)-((E189/E150*H189)+(E190/E150*H190)+(E191/E150*H191)+(E192/E150*H192))</f>
         <v>4.2923216783448237E-2</v>
       </c>
@@ -27370,112 +27421,112 @@
       <c r="K188" s="55"/>
     </row>
     <row r="189" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B189" s="19"/>
-      <c r="C189" s="19"/>
-      <c r="D189" s="21" t="s">
+      <c r="B189" s="59"/>
+      <c r="C189" s="59"/>
+      <c r="D189" s="63" t="s">
         <v>174</v>
       </c>
-      <c r="E189" s="19">
+      <c r="E189" s="59">
         <v>20</v>
       </c>
-      <c r="F189" s="19">
+      <c r="F189" s="59">
         <v>1</v>
       </c>
-      <c r="G189" s="19">
+      <c r="G189" s="59">
         <f t="shared" ref="G189:G192" si="30">E189-F189</f>
         <v>19</v>
       </c>
-      <c r="H189" s="19">
+      <c r="H189" s="59">
         <f t="shared" ref="H189:H192" si="31">((-F189/E189)*IMLOG2(F189/E189)+(-G189/E189)*IMLOG2(G189/E189))</f>
         <v>0.28639695711595603</v>
       </c>
-      <c r="I189" s="19"/>
+      <c r="I189" s="59"/>
       <c r="J189" s="26"/>
       <c r="K189" s="55"/>
     </row>
     <row r="190" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B190" s="19"/>
-      <c r="C190" s="19"/>
-      <c r="D190" s="21" t="s">
+      <c r="B190" s="59"/>
+      <c r="C190" s="59"/>
+      <c r="D190" s="63" t="s">
         <v>175</v>
       </c>
-      <c r="E190" s="19">
+      <c r="E190" s="59">
         <v>32</v>
       </c>
-      <c r="F190" s="19">
+      <c r="F190" s="59">
         <v>9</v>
       </c>
-      <c r="G190" s="19">
+      <c r="G190" s="59">
         <f t="shared" si="30"/>
         <v>23</v>
       </c>
-      <c r="H190" s="19">
+      <c r="H190" s="59">
         <f t="shared" si="31"/>
         <v>0.85714843742837221</v>
       </c>
-      <c r="I190" s="19"/>
+      <c r="I190" s="59"/>
       <c r="J190" s="26"/>
       <c r="K190" s="55"/>
     </row>
     <row r="191" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B191" s="19"/>
-      <c r="C191" s="19"/>
-      <c r="D191" s="21" t="s">
+      <c r="B191" s="59"/>
+      <c r="C191" s="59"/>
+      <c r="D191" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="E191" s="19">
+      <c r="E191" s="59">
         <v>31</v>
       </c>
-      <c r="F191" s="19">
+      <c r="F191" s="59">
         <v>6</v>
       </c>
-      <c r="G191" s="19">
+      <c r="G191" s="59">
         <f t="shared" si="30"/>
         <v>25</v>
       </c>
-      <c r="H191" s="19">
+      <c r="H191" s="59">
         <f t="shared" si="31"/>
         <v>0.70883567333219655</v>
       </c>
-      <c r="I191" s="19"/>
+      <c r="I191" s="59"/>
       <c r="J191" s="26"/>
       <c r="K191" s="55"/>
     </row>
     <row r="192" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B192" s="19"/>
-      <c r="C192" s="19"/>
-      <c r="D192" s="21" t="s">
+      <c r="B192" s="59"/>
+      <c r="C192" s="59"/>
+      <c r="D192" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="E192" s="19">
+      <c r="E192" s="59">
         <v>10</v>
       </c>
-      <c r="F192" s="19">
+      <c r="F192" s="59">
         <v>1</v>
       </c>
-      <c r="G192" s="19">
+      <c r="G192" s="59">
         <f t="shared" si="30"/>
         <v>9</v>
       </c>
-      <c r="H192" s="19">
+      <c r="H192" s="59">
         <f t="shared" si="31"/>
         <v>0.468995593589281</v>
       </c>
-      <c r="I192" s="19"/>
+      <c r="I192" s="59"/>
       <c r="J192" s="26"/>
       <c r="K192" s="55"/>
     </row>
     <row r="193" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B193" s="19"/>
-      <c r="C193" s="19" t="s">
+      <c r="B193" s="59"/>
+      <c r="C193" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="D193" s="19"/>
-      <c r="E193" s="19"/>
-      <c r="F193" s="19"/>
-      <c r="G193" s="19"/>
-      <c r="H193" s="19"/>
-      <c r="I193" s="19">
+      <c r="D193" s="59"/>
+      <c r="E193" s="59"/>
+      <c r="F193" s="59"/>
+      <c r="G193" s="59"/>
+      <c r="H193" s="59"/>
+      <c r="I193" s="59">
         <f>(H150)-((E194/E150*H194)+(E195/E150*H195)+(E196/E150*H196))</f>
         <v>0</v>
       </c>
@@ -27486,70 +27537,70 @@
       <c r="K193" s="55"/>
     </row>
     <row r="194" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B194" s="19"/>
-      <c r="C194" s="19"/>
-      <c r="D194" s="21" t="s">
+      <c r="B194" s="59"/>
+      <c r="C194" s="59"/>
+      <c r="D194" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="E194" s="19">
+      <c r="E194" s="59">
         <v>93</v>
       </c>
-      <c r="F194" s="19">
+      <c r="F194" s="59">
         <v>17</v>
       </c>
-      <c r="G194" s="19">
+      <c r="G194" s="59">
         <f t="shared" ref="G194" si="32">E194-F194</f>
         <v>76</v>
       </c>
-      <c r="H194" s="19">
+      <c r="H194" s="59">
         <f t="shared" ref="H194" si="33">((-F194/E194)*IMLOG2(F194/E194)+(-G194/E194)*IMLOG2(G194/E194))</f>
         <v>0.68615494742020033</v>
       </c>
-      <c r="I194" s="19"/>
+      <c r="I194" s="59"/>
       <c r="J194" s="26"/>
       <c r="K194" s="55"/>
     </row>
     <row r="195" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B195" s="19"/>
-      <c r="C195" s="19"/>
-      <c r="D195" s="21" t="s">
+      <c r="B195" s="59"/>
+      <c r="C195" s="59"/>
+      <c r="D195" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="E195" s="19">
-        <v>0</v>
-      </c>
-      <c r="F195" s="19">
-        <v>0</v>
-      </c>
-      <c r="G195" s="19">
-        <v>0</v>
-      </c>
-      <c r="H195" s="19">
-        <v>0</v>
-      </c>
-      <c r="I195" s="19"/>
+      <c r="E195" s="59">
+        <v>0</v>
+      </c>
+      <c r="F195" s="59">
+        <v>0</v>
+      </c>
+      <c r="G195" s="59">
+        <v>0</v>
+      </c>
+      <c r="H195" s="59">
+        <v>0</v>
+      </c>
+      <c r="I195" s="59"/>
       <c r="J195" s="26"/>
       <c r="K195" s="55"/>
     </row>
     <row r="196" spans="2:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B196" s="19"/>
-      <c r="C196" s="19"/>
-      <c r="D196" s="21" t="s">
+      <c r="B196" s="59"/>
+      <c r="C196" s="59"/>
+      <c r="D196" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="E196" s="19">
-        <v>0</v>
-      </c>
-      <c r="F196" s="19">
-        <v>0</v>
-      </c>
-      <c r="G196" s="19">
-        <v>0</v>
-      </c>
-      <c r="H196" s="19">
-        <v>0</v>
-      </c>
-      <c r="I196" s="19"/>
+      <c r="E196" s="59">
+        <v>0</v>
+      </c>
+      <c r="F196" s="59">
+        <v>0</v>
+      </c>
+      <c r="G196" s="59">
+        <v>0</v>
+      </c>
+      <c r="H196" s="59">
+        <v>0</v>
+      </c>
+      <c r="I196" s="59"/>
       <c r="J196" s="26"/>
       <c r="K196" s="55"/>
     </row>
@@ -27580,44 +27631,44 @@
       </c>
     </row>
     <row r="201" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B201" s="17" t="s">
+      <c r="B201" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="C201" s="23" t="s">
+      <c r="C201" s="65" t="s">
         <v>232</v>
       </c>
-      <c r="D201" s="24"/>
-      <c r="E201" s="24">
+      <c r="D201" s="66"/>
+      <c r="E201" s="66">
         <v>48</v>
       </c>
-      <c r="F201" s="24">
+      <c r="F201" s="66">
         <v>6</v>
       </c>
-      <c r="G201" s="24">
+      <c r="G201" s="66">
         <f t="shared" ref="G201" si="34">E201-F201</f>
         <v>42</v>
       </c>
-      <c r="H201" s="24">
+      <c r="H201" s="66">
         <f>((-F201/E201)*IMLOG2(F201/E201)+(-G201/E201)*IMLOG2(G201/E201))</f>
         <v>0.54356444319959651</v>
       </c>
-      <c r="I201" s="24"/>
+      <c r="I201" s="66"/>
       <c r="J201" s="26"/>
       <c r="K201" s="55" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="202" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B202" s="19"/>
-      <c r="C202" s="19" t="s">
+      <c r="B202" s="67"/>
+      <c r="C202" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="D202" s="19"/>
-      <c r="E202" s="19"/>
-      <c r="F202" s="19"/>
-      <c r="G202" s="19"/>
-      <c r="H202" s="19"/>
-      <c r="I202" s="19">
+      <c r="D202" s="67"/>
+      <c r="E202" s="67"/>
+      <c r="F202" s="67"/>
+      <c r="G202" s="67"/>
+      <c r="H202" s="67"/>
+      <c r="I202" s="67">
         <f>(H201)-((E203/E201*H203)+(E204/E201*H204))</f>
         <v>9.2254391891261056E-3</v>
       </c>
@@ -27628,64 +27679,64 @@
       <c r="K202" s="55"/>
     </row>
     <row r="203" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B203" s="19"/>
-      <c r="C203" s="19"/>
-      <c r="D203" s="19" t="s">
+      <c r="B203" s="67"/>
+      <c r="C203" s="67"/>
+      <c r="D203" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="E203" s="19">
+      <c r="E203" s="67">
         <v>31</v>
       </c>
-      <c r="F203" s="19">
+      <c r="F203" s="67">
         <v>3</v>
       </c>
-      <c r="G203" s="19">
+      <c r="G203" s="67">
         <f>(E203-F203)</f>
         <v>28</v>
       </c>
-      <c r="H203" s="19">
+      <c r="H203" s="67">
         <f t="shared" ref="H203:H204" si="35">((-F203/E203)*IMLOG2(F203/E203)+(-G203/E203)*IMLOG2(G203/E203))</f>
         <v>0.45868581620054028</v>
       </c>
-      <c r="I203" s="19"/>
+      <c r="I203" s="67"/>
       <c r="J203" s="26"/>
       <c r="K203" s="55"/>
     </row>
     <row r="204" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B204" s="19"/>
-      <c r="C204" s="19"/>
-      <c r="D204" s="19" t="s">
+      <c r="B204" s="67"/>
+      <c r="C204" s="67"/>
+      <c r="D204" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="E204" s="19">
+      <c r="E204" s="67">
         <v>17</v>
       </c>
-      <c r="F204" s="19">
+      <c r="F204" s="67">
         <v>3</v>
       </c>
-      <c r="G204" s="19">
+      <c r="G204" s="67">
         <f>(E204-F204)</f>
         <v>14</v>
       </c>
-      <c r="H204" s="19">
+      <c r="H204" s="67">
         <f t="shared" si="35"/>
         <v>0.6722948170756371</v>
       </c>
-      <c r="I204" s="19"/>
+      <c r="I204" s="67"/>
       <c r="J204" s="26"/>
       <c r="K204" s="55"/>
     </row>
     <row r="205" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B205" s="19"/>
-      <c r="C205" s="19" t="s">
+      <c r="B205" s="67"/>
+      <c r="C205" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="D205" s="19"/>
-      <c r="E205" s="19"/>
-      <c r="F205" s="19"/>
-      <c r="G205" s="19"/>
-      <c r="H205" s="19"/>
-      <c r="I205" s="19">
+      <c r="D205" s="67"/>
+      <c r="E205" s="67"/>
+      <c r="F205" s="67"/>
+      <c r="G205" s="67"/>
+      <c r="H205" s="67"/>
+      <c r="I205" s="67">
         <f>(H201)-((E206/E201*H206)+(E207/E201*H207)+(E208/E201*H208))</f>
         <v>0.10630054313156628</v>
       </c>
@@ -27696,86 +27747,86 @@
       <c r="K205" s="55"/>
     </row>
     <row r="206" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B206" s="19"/>
-      <c r="C206" s="19"/>
-      <c r="D206" s="19" t="s">
+      <c r="B206" s="67"/>
+      <c r="C206" s="67"/>
+      <c r="D206" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="E206" s="19">
+      <c r="E206" s="67">
         <v>28</v>
       </c>
-      <c r="F206" s="19">
+      <c r="F206" s="67">
         <v>6</v>
       </c>
-      <c r="G206" s="19">
+      <c r="G206" s="67">
         <f>E206-F206</f>
         <v>22</v>
       </c>
-      <c r="H206" s="19">
+      <c r="H206" s="67">
         <f t="shared" ref="H206" si="37">((-F206/E206)*IMLOG2(F206/E206)+(-G206/E206)*IMLOG2(G206/E206))</f>
         <v>0.7495952572594804</v>
       </c>
-      <c r="I206" s="19"/>
+      <c r="I206" s="67"/>
       <c r="J206" s="26"/>
       <c r="K206" s="55"/>
     </row>
     <row r="207" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B207" s="19"/>
-      <c r="C207" s="19"/>
-      <c r="D207" s="19" t="s">
+      <c r="B207" s="67"/>
+      <c r="C207" s="67"/>
+      <c r="D207" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="E207" s="19">
+      <c r="E207" s="67">
         <v>14</v>
       </c>
-      <c r="F207" s="19">
-        <v>0</v>
-      </c>
-      <c r="G207" s="19">
+      <c r="F207" s="67">
+        <v>0</v>
+      </c>
+      <c r="G207" s="67">
         <f t="shared" ref="G207:G208" si="38">E207-F207</f>
         <v>14</v>
       </c>
-      <c r="H207" s="19">
-        <v>0</v>
-      </c>
-      <c r="I207" s="19"/>
+      <c r="H207" s="67">
+        <v>0</v>
+      </c>
+      <c r="I207" s="67"/>
       <c r="J207" s="26"/>
       <c r="K207" s="55"/>
     </row>
     <row r="208" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B208" s="19"/>
-      <c r="C208" s="19"/>
-      <c r="D208" s="19" t="s">
+      <c r="B208" s="67"/>
+      <c r="C208" s="67"/>
+      <c r="D208" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="E208" s="19">
+      <c r="E208" s="67">
         <v>6</v>
       </c>
-      <c r="F208" s="19">
-        <v>0</v>
-      </c>
-      <c r="G208" s="19">
+      <c r="F208" s="67">
+        <v>0</v>
+      </c>
+      <c r="G208" s="67">
         <f t="shared" si="38"/>
         <v>6</v>
       </c>
-      <c r="H208" s="19">
-        <v>0</v>
-      </c>
-      <c r="I208" s="19"/>
+      <c r="H208" s="67">
+        <v>0</v>
+      </c>
+      <c r="I208" s="67"/>
       <c r="J208" s="26"/>
       <c r="K208" s="55"/>
     </row>
     <row r="209" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B209" s="39"/>
-      <c r="C209" s="39" t="s">
+      <c r="B209" s="68"/>
+      <c r="C209" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="D209" s="39"/>
-      <c r="E209" s="39"/>
-      <c r="F209" s="39"/>
-      <c r="G209" s="39"/>
-      <c r="H209" s="39"/>
-      <c r="I209" s="39">
+      <c r="D209" s="68"/>
+      <c r="E209" s="68"/>
+      <c r="F209" s="68"/>
+      <c r="G209" s="68"/>
+      <c r="H209" s="68"/>
+      <c r="I209" s="68">
         <f>(H201)-((E210/E201*H210)+(E211/E201*H211)+(E212/E201*H212)+(E213/E201*H213))</f>
         <v>0.17635990185347417</v>
       </c>
@@ -27785,118 +27836,118 @@
       </c>
       <c r="K209" s="55"/>
     </row>
-    <row r="210" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B210" s="39"/>
-      <c r="C210" s="39"/>
-      <c r="D210" s="40" t="s">
+    <row r="210" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B210" s="68"/>
+      <c r="C210" s="68"/>
+      <c r="D210" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E210" s="48">
+      <c r="E210" s="70">
         <v>6</v>
       </c>
-      <c r="F210" s="48">
-        <v>0</v>
-      </c>
-      <c r="G210" s="48">
+      <c r="F210" s="70">
+        <v>0</v>
+      </c>
+      <c r="G210" s="70">
         <f t="shared" ref="G210:G213" si="39">E210-F210</f>
         <v>6</v>
       </c>
-      <c r="H210" s="48">
-        <v>0</v>
-      </c>
-      <c r="I210" s="39"/>
+      <c r="H210" s="70">
+        <v>0</v>
+      </c>
+      <c r="I210" s="68"/>
       <c r="J210" s="50" t="s">
         <v>26</v>
       </c>
       <c r="K210" s="55"/>
     </row>
     <row r="211" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B211" s="39"/>
-      <c r="C211" s="39"/>
-      <c r="D211" s="39" t="s">
+      <c r="B211" s="68"/>
+      <c r="C211" s="68"/>
+      <c r="D211" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="E211" s="48">
+      <c r="E211" s="70">
         <v>5</v>
       </c>
-      <c r="F211" s="48">
-        <v>0</v>
-      </c>
-      <c r="G211" s="48">
+      <c r="F211" s="70">
+        <v>0</v>
+      </c>
+      <c r="G211" s="70">
         <f t="shared" si="39"/>
         <v>5</v>
       </c>
-      <c r="H211" s="48">
-        <v>0</v>
-      </c>
-      <c r="I211" s="39"/>
+      <c r="H211" s="70">
+        <v>0</v>
+      </c>
+      <c r="I211" s="68"/>
       <c r="J211" s="50" t="s">
         <v>26</v>
       </c>
       <c r="K211" s="55"/>
     </row>
-    <row r="212" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B212" s="39"/>
-      <c r="C212" s="39"/>
-      <c r="D212" s="40" t="s">
+    <row r="212" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B212" s="68"/>
+      <c r="C212" s="68"/>
+      <c r="D212" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="E212" s="48">
+      <c r="E212" s="70">
         <v>20</v>
       </c>
-      <c r="F212" s="48">
+      <c r="F212" s="70">
         <v>6</v>
       </c>
-      <c r="G212" s="48">
+      <c r="G212" s="70">
         <f t="shared" si="39"/>
         <v>14</v>
       </c>
-      <c r="H212" s="48">
+      <c r="H212" s="70">
         <f t="shared" ref="H212" si="40">((-F212/E212)*IMLOG2(F212/E212)+(-G212/E212)*IMLOG2(G212/E212))</f>
         <v>0.88129089923069359</v>
       </c>
-      <c r="I212" s="39"/>
+      <c r="I212" s="68"/>
       <c r="J212" s="50" t="s">
         <v>229</v>
       </c>
       <c r="K212" s="55"/>
     </row>
-    <row r="213" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B213" s="39"/>
-      <c r="C213" s="39"/>
-      <c r="D213" s="40" t="s">
+    <row r="213" spans="2:11" ht="23" x14ac:dyDescent="0.45">
+      <c r="B213" s="68"/>
+      <c r="C213" s="68"/>
+      <c r="D213" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="E213" s="48">
+      <c r="E213" s="70">
         <v>17</v>
       </c>
-      <c r="F213" s="48">
-        <v>0</v>
-      </c>
-      <c r="G213" s="48">
+      <c r="F213" s="70">
+        <v>0</v>
+      </c>
+      <c r="G213" s="70">
         <f t="shared" si="39"/>
         <v>17</v>
       </c>
-      <c r="H213" s="48">
-        <v>0</v>
-      </c>
-      <c r="I213" s="39"/>
+      <c r="H213" s="70">
+        <v>0</v>
+      </c>
+      <c r="I213" s="68"/>
       <c r="J213" s="50" t="s">
         <v>26</v>
       </c>
       <c r="K213" s="55"/>
     </row>
-    <row r="214" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B214" s="19"/>
-      <c r="C214" s="21" t="s">
+    <row r="214" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B214" s="67"/>
+      <c r="C214" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="D214" s="19"/>
-      <c r="E214" s="19"/>
-      <c r="F214" s="19"/>
-      <c r="G214" s="19"/>
-      <c r="H214" s="19"/>
-      <c r="I214" s="19">
+      <c r="D214" s="67"/>
+      <c r="E214" s="67"/>
+      <c r="F214" s="67"/>
+      <c r="G214" s="67"/>
+      <c r="H214" s="67"/>
+      <c r="I214" s="67">
         <f>(H201)-((E215/E201*H215)+(E216/E201*H216)+(E217/E201*H217))</f>
         <v>9.071146058272983E-2</v>
       </c>
@@ -27907,88 +27958,88 @@
       <c r="K214" s="55"/>
     </row>
     <row r="215" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B215" s="19"/>
-      <c r="C215" s="19"/>
-      <c r="D215" s="21" t="s">
+      <c r="B215" s="67"/>
+      <c r="C215" s="67"/>
+      <c r="D215" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="E215" s="19">
+      <c r="E215" s="67">
         <v>3</v>
       </c>
-      <c r="F215" s="19">
+      <c r="F215" s="67">
         <v>2</v>
       </c>
-      <c r="G215" s="19">
+      <c r="G215" s="67">
         <f t="shared" ref="G215:G217" si="41">E215-F215</f>
         <v>1</v>
       </c>
-      <c r="H215" s="19">
+      <c r="H215" s="67">
         <f t="shared" ref="H215:H217" si="42">((-F215/E215)*IMLOG2(F215/E215)+(-G215/E215)*IMLOG2(G215/E215))</f>
         <v>0.91829583405449056</v>
       </c>
-      <c r="I215" s="19"/>
+      <c r="I215" s="67"/>
       <c r="J215" s="26"/>
       <c r="K215" s="55"/>
     </row>
     <row r="216" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B216" s="19"/>
-      <c r="C216" s="19"/>
-      <c r="D216" s="21" t="s">
+      <c r="B216" s="67"/>
+      <c r="C216" s="67"/>
+      <c r="D216" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="E216" s="19">
+      <c r="E216" s="67">
         <v>31</v>
       </c>
-      <c r="F216" s="19">
+      <c r="F216" s="67">
         <v>2</v>
       </c>
-      <c r="G216" s="19">
+      <c r="G216" s="67">
         <f t="shared" si="41"/>
         <v>29</v>
       </c>
-      <c r="H216" s="19">
+      <c r="H216" s="67">
         <f t="shared" si="42"/>
         <v>0.34511731494495329</v>
       </c>
-      <c r="I216" s="19"/>
+      <c r="I216" s="67"/>
       <c r="J216" s="26"/>
       <c r="K216" s="55"/>
     </row>
     <row r="217" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B217" s="19"/>
-      <c r="C217" s="19"/>
-      <c r="D217" s="21" t="s">
+      <c r="B217" s="67"/>
+      <c r="C217" s="67"/>
+      <c r="D217" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="E217" s="19">
+      <c r="E217" s="67">
         <v>14</v>
       </c>
-      <c r="F217" s="19">
+      <c r="F217" s="67">
         <v>2</v>
       </c>
-      <c r="G217" s="19">
+      <c r="G217" s="67">
         <f t="shared" si="41"/>
         <v>12</v>
       </c>
-      <c r="H217" s="19">
+      <c r="H217" s="67">
         <f t="shared" si="42"/>
         <v>0.59167277858232681</v>
       </c>
-      <c r="I217" s="19"/>
+      <c r="I217" s="67"/>
       <c r="J217" s="26"/>
       <c r="K217" s="55"/>
     </row>
     <row r="218" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B218" s="19"/>
-      <c r="C218" s="19" t="s">
+      <c r="B218" s="67"/>
+      <c r="C218" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="D218" s="19"/>
-      <c r="E218" s="19"/>
-      <c r="F218" s="19"/>
-      <c r="G218" s="19"/>
-      <c r="H218" s="19"/>
-      <c r="I218" s="19">
+      <c r="D218" s="67"/>
+      <c r="E218" s="67"/>
+      <c r="F218" s="67"/>
+      <c r="G218" s="67"/>
+      <c r="H218" s="67"/>
+      <c r="I218" s="67">
         <f>(H201)-((E219/E201*H219)+(E220/E201*H220)+(E221/E201*H221))</f>
         <v>0.10481383183877757</v>
       </c>
@@ -27999,87 +28050,87 @@
       <c r="K218" s="55"/>
     </row>
     <row r="219" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B219" s="19"/>
-      <c r="C219" s="19"/>
-      <c r="D219" s="21" t="s">
+      <c r="B219" s="67"/>
+      <c r="C219" s="67"/>
+      <c r="D219" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="E219" s="19">
+      <c r="E219" s="67">
         <v>20</v>
       </c>
-      <c r="F219" s="19">
+      <c r="F219" s="67">
         <v>5</v>
       </c>
-      <c r="G219" s="19">
+      <c r="G219" s="67">
         <f t="shared" ref="G219:G221" si="43">E219-F219</f>
         <v>15</v>
       </c>
-      <c r="H219" s="19">
+      <c r="H219" s="67">
         <f>((-F219/E219)*IMLOG2(F219/E219)+(-G219/E219)*IMLOG2(G219/E219))</f>
         <v>0.81127812445913294</v>
       </c>
-      <c r="I219" s="19"/>
+      <c r="I219" s="67"/>
       <c r="J219" s="26"/>
       <c r="K219" s="55"/>
     </row>
     <row r="220" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B220" s="19"/>
-      <c r="C220" s="19"/>
-      <c r="D220" s="21" t="s">
+      <c r="B220" s="67"/>
+      <c r="C220" s="67"/>
+      <c r="D220" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="E220" s="19">
+      <c r="E220" s="67">
         <v>11</v>
       </c>
-      <c r="F220" s="19">
+      <c r="F220" s="67">
         <v>1</v>
       </c>
-      <c r="G220" s="19">
+      <c r="G220" s="67">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="H220" s="19">
+      <c r="H220" s="67">
         <f t="shared" ref="H220" si="44">((-F220/E220)*IMLOG2(F220/E220)+(-G220/E220)*IMLOG2(G220/E220))</f>
         <v>0.43949698692151362</v>
       </c>
-      <c r="I220" s="19"/>
+      <c r="I220" s="67"/>
       <c r="J220" s="26"/>
       <c r="K220" s="55"/>
     </row>
     <row r="221" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B221" s="19"/>
-      <c r="C221" s="19"/>
-      <c r="D221" s="21" t="s">
+      <c r="B221" s="67"/>
+      <c r="C221" s="67"/>
+      <c r="D221" s="71" t="s">
         <v>169</v>
       </c>
-      <c r="E221" s="19">
+      <c r="E221" s="67">
         <v>17</v>
       </c>
-      <c r="F221" s="19">
-        <v>0</v>
-      </c>
-      <c r="G221" s="19">
+      <c r="F221" s="67">
+        <v>0</v>
+      </c>
+      <c r="G221" s="67">
         <f t="shared" si="43"/>
         <v>17</v>
       </c>
-      <c r="H221" s="19">
-        <v>0</v>
-      </c>
-      <c r="I221" s="19"/>
+      <c r="H221" s="67">
+        <v>0</v>
+      </c>
+      <c r="I221" s="67"/>
       <c r="J221" s="26"/>
       <c r="K221" s="55"/>
     </row>
-    <row r="222" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B222" s="19"/>
-      <c r="C222" s="21" t="s">
+    <row r="222" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B222" s="67"/>
+      <c r="C222" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="D222" s="19"/>
-      <c r="E222" s="19"/>
-      <c r="F222" s="19"/>
-      <c r="G222" s="19"/>
-      <c r="H222" s="19"/>
-      <c r="I222" s="19">
+      <c r="D222" s="67"/>
+      <c r="E222" s="67"/>
+      <c r="F222" s="67"/>
+      <c r="G222" s="67"/>
+      <c r="H222" s="67"/>
+      <c r="I222" s="67">
         <f>(H201)-((E223/E201*H223)+(E224/E201*H224))</f>
         <v>8.5665298173588367E-3</v>
       </c>
@@ -28090,64 +28141,64 @@
       <c r="K222" s="55"/>
     </row>
     <row r="223" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B223" s="19"/>
-      <c r="C223" s="19"/>
-      <c r="D223" s="21" t="s">
+      <c r="B223" s="67"/>
+      <c r="C223" s="67"/>
+      <c r="D223" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="E223" s="19">
+      <c r="E223" s="67">
         <v>14</v>
       </c>
-      <c r="F223" s="19">
+      <c r="F223" s="67">
         <v>1</v>
       </c>
-      <c r="G223" s="19">
+      <c r="G223" s="67">
         <f t="shared" ref="G223:G224" si="45">E223-F223</f>
         <v>13</v>
       </c>
-      <c r="H223" s="19">
+      <c r="H223" s="67">
         <f>((-F223/E223)*IMLOG2(F223/E223)+(-G223/E223)*IMLOG2(G223/E223))</f>
         <v>0.37123232664087613</v>
       </c>
-      <c r="I223" s="19"/>
+      <c r="I223" s="67"/>
       <c r="J223" s="26"/>
       <c r="K223" s="55"/>
     </row>
     <row r="224" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B224" s="19"/>
-      <c r="C224" s="19"/>
-      <c r="D224" s="21" t="s">
+      <c r="B224" s="67"/>
+      <c r="C224" s="67"/>
+      <c r="D224" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="E224" s="19">
+      <c r="E224" s="67">
         <v>34</v>
       </c>
-      <c r="F224" s="19">
+      <c r="F224" s="67">
         <v>5</v>
       </c>
-      <c r="G224" s="19">
+      <c r="G224" s="67">
         <f t="shared" si="45"/>
         <v>29</v>
       </c>
-      <c r="H224" s="19">
+      <c r="H224" s="67">
         <f t="shared" ref="H224" si="46">((-F224/E224)*IMLOG2(F224/E224)+(-G224/E224)*IMLOG2(G224/E224))</f>
         <v>0.60243080204044541</v>
       </c>
-      <c r="I224" s="19"/>
+      <c r="I224" s="67"/>
       <c r="J224" s="26"/>
       <c r="K224" s="55"/>
     </row>
-    <row r="225" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B225" s="19"/>
-      <c r="C225" s="21" t="s">
+    <row r="225" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B225" s="67"/>
+      <c r="C225" s="71" t="s">
         <v>171</v>
       </c>
-      <c r="D225" s="19"/>
-      <c r="E225" s="19"/>
-      <c r="F225" s="19"/>
-      <c r="G225" s="19"/>
-      <c r="H225" s="19"/>
-      <c r="I225" s="19">
+      <c r="D225" s="67"/>
+      <c r="E225" s="67"/>
+      <c r="F225" s="67"/>
+      <c r="G225" s="67"/>
+      <c r="H225" s="67"/>
+      <c r="I225" s="67">
         <f>(H201)-((E226/E201*H226)+(E227/E201*H227)+(E228/E201*H228))</f>
         <v>1.7775437712883146E-2</v>
       </c>
@@ -28158,87 +28209,87 @@
       <c r="K225" s="55"/>
     </row>
     <row r="226" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B226" s="19"/>
-      <c r="C226" s="19"/>
-      <c r="D226" s="21" t="s">
+      <c r="B226" s="67"/>
+      <c r="C226" s="67"/>
+      <c r="D226" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="E226" s="19">
+      <c r="E226" s="67">
         <v>35</v>
       </c>
-      <c r="F226" s="19">
+      <c r="F226" s="67">
         <v>5</v>
       </c>
-      <c r="G226" s="19">
+      <c r="G226" s="67">
         <f t="shared" ref="G226:G228" si="47">E226-F226</f>
         <v>30</v>
       </c>
-      <c r="H226" s="19">
+      <c r="H226" s="67">
         <f t="shared" ref="H226:H227" si="48">((-F226/E226)*IMLOG2(F226/E226)+(-G226/E226)*IMLOG2(G226/E226))</f>
         <v>0.59167277858232681</v>
       </c>
-      <c r="I226" s="19"/>
+      <c r="I226" s="67"/>
       <c r="J226" s="26"/>
       <c r="K226" s="55"/>
     </row>
     <row r="227" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B227" s="19"/>
-      <c r="C227" s="19"/>
-      <c r="D227" s="21" t="s">
+      <c r="B227" s="67"/>
+      <c r="C227" s="67"/>
+      <c r="D227" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="E227" s="19">
+      <c r="E227" s="67">
         <v>9</v>
       </c>
-      <c r="F227" s="19">
+      <c r="F227" s="67">
         <v>1</v>
       </c>
-      <c r="G227" s="19">
+      <c r="G227" s="67">
         <f t="shared" si="47"/>
         <v>8</v>
       </c>
-      <c r="H227" s="19">
+      <c r="H227" s="67">
         <f t="shared" si="48"/>
         <v>0.50325833477564508</v>
       </c>
-      <c r="I227" s="19"/>
+      <c r="I227" s="67"/>
       <c r="J227" s="26"/>
       <c r="K227" s="55"/>
     </row>
     <row r="228" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B228" s="19"/>
-      <c r="C228" s="19"/>
-      <c r="D228" s="21" t="s">
+      <c r="B228" s="67"/>
+      <c r="C228" s="67"/>
+      <c r="D228" s="71" t="s">
         <v>220</v>
       </c>
-      <c r="E228" s="19">
+      <c r="E228" s="67">
         <v>4</v>
       </c>
-      <c r="F228" s="19">
-        <v>0</v>
-      </c>
-      <c r="G228" s="19">
+      <c r="F228" s="67">
+        <v>0</v>
+      </c>
+      <c r="G228" s="67">
         <f t="shared" si="47"/>
         <v>4</v>
       </c>
-      <c r="H228" s="19">
-        <v>0</v>
-      </c>
-      <c r="I228" s="19"/>
+      <c r="H228" s="67">
+        <v>0</v>
+      </c>
+      <c r="I228" s="67"/>
       <c r="J228" s="26"/>
       <c r="K228" s="55"/>
     </row>
-    <row r="229" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B229" s="19"/>
-      <c r="C229" s="21" t="s">
+    <row r="229" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B229" s="67"/>
+      <c r="C229" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="D229" s="19"/>
-      <c r="E229" s="19"/>
-      <c r="F229" s="19"/>
-      <c r="G229" s="19"/>
-      <c r="H229" s="19"/>
-      <c r="I229" s="19">
+      <c r="D229" s="67"/>
+      <c r="E229" s="67"/>
+      <c r="F229" s="67"/>
+      <c r="G229" s="67"/>
+      <c r="H229" s="67"/>
+      <c r="I229" s="67">
         <f>(H201)-((E230/E201*H230)+(E231/E201*H231)+(E232/E201*H232)+(E233/E201*H233))</f>
         <v>7.328801869775492E-2</v>
       </c>
@@ -28249,109 +28300,109 @@
       <c r="K229" s="55"/>
     </row>
     <row r="230" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B230" s="19"/>
-      <c r="C230" s="19"/>
-      <c r="D230" s="21" t="s">
+      <c r="B230" s="67"/>
+      <c r="C230" s="67"/>
+      <c r="D230" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="E230" s="19">
+      <c r="E230" s="67">
         <v>9</v>
       </c>
-      <c r="F230" s="19">
-        <v>0</v>
-      </c>
-      <c r="G230" s="19">
+      <c r="F230" s="67">
+        <v>0</v>
+      </c>
+      <c r="G230" s="67">
         <f t="shared" ref="G230:G233" si="49">E230-F230</f>
         <v>9</v>
       </c>
-      <c r="H230" s="19">
-        <v>0</v>
-      </c>
-      <c r="I230" s="19"/>
+      <c r="H230" s="67">
+        <v>0</v>
+      </c>
+      <c r="I230" s="67"/>
       <c r="J230" s="26"/>
       <c r="K230" s="55"/>
     </row>
     <row r="231" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B231" s="19"/>
-      <c r="C231" s="19"/>
-      <c r="D231" s="21" t="s">
+      <c r="B231" s="67"/>
+      <c r="C231" s="67"/>
+      <c r="D231" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="E231" s="19">
+      <c r="E231" s="67">
         <v>1</v>
       </c>
-      <c r="F231" s="19">
-        <v>0</v>
-      </c>
-      <c r="G231" s="19">
+      <c r="F231" s="67">
+        <v>0</v>
+      </c>
+      <c r="G231" s="67">
         <f t="shared" si="49"/>
         <v>1</v>
       </c>
-      <c r="H231" s="19">
-        <v>0</v>
-      </c>
-      <c r="I231" s="19"/>
+      <c r="H231" s="67">
+        <v>0</v>
+      </c>
+      <c r="I231" s="67"/>
       <c r="J231" s="26"/>
       <c r="K231" s="55"/>
     </row>
     <row r="232" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B232" s="19"/>
-      <c r="C232" s="19"/>
-      <c r="D232" s="21" t="s">
+      <c r="B232" s="67"/>
+      <c r="C232" s="67"/>
+      <c r="D232" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="E232" s="19">
+      <c r="E232" s="67">
         <v>5</v>
       </c>
-      <c r="F232" s="19">
-        <v>0</v>
-      </c>
-      <c r="G232" s="19">
+      <c r="F232" s="67">
+        <v>0</v>
+      </c>
+      <c r="G232" s="67">
         <f t="shared" si="49"/>
         <v>5</v>
       </c>
-      <c r="H232" s="19">
-        <v>0</v>
-      </c>
-      <c r="I232" s="19"/>
+      <c r="H232" s="67">
+        <v>0</v>
+      </c>
+      <c r="I232" s="67"/>
       <c r="J232" s="26"/>
       <c r="K232" s="55"/>
     </row>
     <row r="233" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B233" s="19"/>
-      <c r="C233" s="19"/>
-      <c r="D233" s="21" t="s">
+      <c r="B233" s="67"/>
+      <c r="C233" s="67"/>
+      <c r="D233" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="E233" s="19">
+      <c r="E233" s="67">
         <v>33</v>
       </c>
-      <c r="F233" s="19">
+      <c r="F233" s="67">
         <v>6</v>
       </c>
-      <c r="G233" s="19">
+      <c r="G233" s="67">
         <f t="shared" si="49"/>
         <v>27</v>
       </c>
-      <c r="H233" s="19">
+      <c r="H233" s="67">
         <f t="shared" ref="H233" si="50">((-F233/E233)*IMLOG2(F233/E233)+(-G233/E233)*IMLOG2(G233/E233))</f>
         <v>0.68403843563904232</v>
       </c>
-      <c r="I233" s="19"/>
+      <c r="I233" s="67"/>
       <c r="J233" s="26"/>
       <c r="K233" s="55"/>
     </row>
-    <row r="234" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B234" s="19"/>
-      <c r="C234" s="21" t="s">
+    <row r="234" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B234" s="67"/>
+      <c r="C234" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="D234" s="19"/>
-      <c r="E234" s="19"/>
-      <c r="F234" s="19"/>
-      <c r="G234" s="19"/>
-      <c r="H234" s="19"/>
-      <c r="I234" s="19">
+      <c r="D234" s="67"/>
+      <c r="E234" s="67"/>
+      <c r="F234" s="67"/>
+      <c r="G234" s="67"/>
+      <c r="H234" s="67"/>
+      <c r="I234" s="67">
         <f>(H201)-((E235/E201*H235)+(E236/E201*H236)+(E237/E201*H237)+(E238/E201*H238))</f>
         <v>0.12045828863013358</v>
       </c>
@@ -28362,110 +28413,110 @@
       <c r="K234" s="55"/>
     </row>
     <row r="235" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B235" s="19"/>
-      <c r="C235" s="19"/>
-      <c r="D235" s="21" t="s">
+      <c r="B235" s="67"/>
+      <c r="C235" s="67"/>
+      <c r="D235" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="E235" s="19">
+      <c r="E235" s="67">
         <v>12</v>
       </c>
-      <c r="F235" s="19">
-        <v>0</v>
-      </c>
-      <c r="G235" s="19">
+      <c r="F235" s="67">
+        <v>0</v>
+      </c>
+      <c r="G235" s="67">
         <f t="shared" ref="G235:G238" si="51">E235-F235</f>
         <v>12</v>
       </c>
-      <c r="H235" s="19">
-        <v>0</v>
-      </c>
-      <c r="I235" s="19"/>
+      <c r="H235" s="67">
+        <v>0</v>
+      </c>
+      <c r="I235" s="67"/>
       <c r="J235" s="26"/>
       <c r="K235" s="55"/>
     </row>
     <row r="236" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B236" s="19"/>
-      <c r="C236" s="19"/>
-      <c r="D236" s="21" t="s">
+      <c r="B236" s="67"/>
+      <c r="C236" s="67"/>
+      <c r="D236" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="E236" s="19">
+      <c r="E236" s="67">
         <v>18</v>
       </c>
-      <c r="F236" s="19">
+      <c r="F236" s="67">
         <v>5</v>
       </c>
-      <c r="G236" s="19">
+      <c r="G236" s="67">
         <f t="shared" si="51"/>
         <v>13</v>
       </c>
-      <c r="H236" s="19">
+      <c r="H236" s="67">
         <f t="shared" ref="H236:H237" si="52">((-F236/E236)*IMLOG2(F236/E236)+(-G236/E236)*IMLOG2(G236/E236))</f>
         <v>0.8524051786494784</v>
       </c>
-      <c r="I236" s="19"/>
+      <c r="I236" s="67"/>
       <c r="J236" s="26"/>
       <c r="K236" s="55"/>
     </row>
     <row r="237" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B237" s="19"/>
-      <c r="C237" s="19"/>
-      <c r="D237" s="21" t="s">
+      <c r="B237" s="67"/>
+      <c r="C237" s="67"/>
+      <c r="D237" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="E237" s="19">
+      <c r="E237" s="67">
         <v>12</v>
       </c>
-      <c r="F237" s="19">
+      <c r="F237" s="67">
         <v>1</v>
       </c>
-      <c r="G237" s="19">
+      <c r="G237" s="67">
         <f t="shared" si="51"/>
         <v>11</v>
       </c>
-      <c r="H237" s="19">
+      <c r="H237" s="67">
         <f t="shared" si="52"/>
         <v>0.41381685030363408</v>
       </c>
-      <c r="I237" s="19"/>
+      <c r="I237" s="67"/>
       <c r="J237" s="26"/>
       <c r="K237" s="55"/>
     </row>
     <row r="238" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
-      <c r="D238" s="21" t="s">
+      <c r="B238" s="67"/>
+      <c r="C238" s="67"/>
+      <c r="D238" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="E238" s="19">
+      <c r="E238" s="67">
         <v>6</v>
       </c>
-      <c r="F238" s="19">
-        <v>0</v>
-      </c>
-      <c r="G238" s="19">
+      <c r="F238" s="67">
+        <v>0</v>
+      </c>
+      <c r="G238" s="67">
         <f t="shared" si="51"/>
         <v>6</v>
       </c>
-      <c r="H238" s="19">
-        <v>0</v>
-      </c>
-      <c r="I238" s="19"/>
+      <c r="H238" s="67">
+        <v>0</v>
+      </c>
+      <c r="I238" s="67"/>
       <c r="J238" s="26"/>
       <c r="K238" s="55"/>
     </row>
     <row r="239" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B239" s="19"/>
-      <c r="C239" s="19" t="s">
+      <c r="B239" s="67"/>
+      <c r="C239" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="D239" s="19"/>
-      <c r="E239" s="19"/>
-      <c r="F239" s="19"/>
-      <c r="G239" s="19"/>
-      <c r="H239" s="19"/>
-      <c r="I239" s="19">
+      <c r="D239" s="67"/>
+      <c r="E239" s="67"/>
+      <c r="F239" s="67"/>
+      <c r="G239" s="67"/>
+      <c r="H239" s="67"/>
+      <c r="I239" s="67">
         <f>(H201)-((E240/E201*H240)+(E241/E201*H241)+(E242/E201*H242))</f>
         <v>0</v>
       </c>
@@ -28476,70 +28527,70 @@
       <c r="K239" s="55"/>
     </row>
     <row r="240" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B240" s="19"/>
-      <c r="C240" s="19"/>
-      <c r="D240" s="21" t="s">
+      <c r="B240" s="67"/>
+      <c r="C240" s="67"/>
+      <c r="D240" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="E240" s="19">
+      <c r="E240" s="67">
         <v>48</v>
       </c>
-      <c r="F240" s="19">
+      <c r="F240" s="67">
         <v>6</v>
       </c>
-      <c r="G240" s="19">
+      <c r="G240" s="67">
         <f t="shared" ref="G240" si="53">E240-F240</f>
         <v>42</v>
       </c>
-      <c r="H240" s="19">
+      <c r="H240" s="67">
         <f t="shared" ref="H240" si="54">((-F240/E240)*IMLOG2(F240/E240)+(-G240/E240)*IMLOG2(G240/E240))</f>
         <v>0.54356444319959651</v>
       </c>
-      <c r="I240" s="19"/>
+      <c r="I240" s="67"/>
       <c r="J240" s="26"/>
       <c r="K240" s="55"/>
     </row>
     <row r="241" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B241" s="19"/>
-      <c r="C241" s="19"/>
-      <c r="D241" s="21" t="s">
+      <c r="B241" s="67"/>
+      <c r="C241" s="67"/>
+      <c r="D241" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="E241" s="19">
-        <v>0</v>
-      </c>
-      <c r="F241" s="19">
-        <v>0</v>
-      </c>
-      <c r="G241" s="19">
-        <v>0</v>
-      </c>
-      <c r="H241" s="19">
-        <v>0</v>
-      </c>
-      <c r="I241" s="19"/>
+      <c r="E241" s="67">
+        <v>0</v>
+      </c>
+      <c r="F241" s="67">
+        <v>0</v>
+      </c>
+      <c r="G241" s="67">
+        <v>0</v>
+      </c>
+      <c r="H241" s="67">
+        <v>0</v>
+      </c>
+      <c r="I241" s="67"/>
       <c r="J241" s="26"/>
       <c r="K241" s="55"/>
     </row>
     <row r="242" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B242" s="19"/>
-      <c r="C242" s="19"/>
-      <c r="D242" s="21" t="s">
+      <c r="B242" s="67"/>
+      <c r="C242" s="67"/>
+      <c r="D242" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="E242" s="19">
-        <v>0</v>
-      </c>
-      <c r="F242" s="19">
-        <v>0</v>
-      </c>
-      <c r="G242" s="19">
-        <v>0</v>
-      </c>
-      <c r="H242" s="19">
-        <v>0</v>
-      </c>
-      <c r="I242" s="19"/>
+      <c r="E242" s="67">
+        <v>0</v>
+      </c>
+      <c r="F242" s="67">
+        <v>0</v>
+      </c>
+      <c r="G242" s="67">
+        <v>0</v>
+      </c>
+      <c r="H242" s="67">
+        <v>0</v>
+      </c>
+      <c r="I242" s="67"/>
       <c r="J242" s="26"/>
       <c r="K242" s="55"/>
     </row>
@@ -32312,45 +32363,45 @@
         <v>222</v>
       </c>
     </row>
-    <row r="421" spans="2:11" ht="31" x14ac:dyDescent="0.45">
-      <c r="B421" s="17" t="s">
+    <row r="421" spans="2:11" ht="21" x14ac:dyDescent="0.45">
+      <c r="B421" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="C421" s="23" t="s">
+      <c r="C421" s="65" t="s">
         <v>241</v>
       </c>
-      <c r="D421" s="24"/>
-      <c r="E421" s="24">
+      <c r="D421" s="66"/>
+      <c r="E421" s="66">
         <v>5</v>
       </c>
-      <c r="F421" s="24">
+      <c r="F421" s="66">
         <v>2</v>
       </c>
-      <c r="G421" s="24">
+      <c r="G421" s="66">
         <f>E421-F421</f>
         <v>3</v>
       </c>
-      <c r="H421" s="24">
+      <c r="H421" s="66">
         <f>((-F421/E421)*IMLOG2(F421/E421)+(-G421/E421)*IMLOG2(G421/E421))</f>
         <v>0.97095059445466747</v>
       </c>
-      <c r="I421" s="24"/>
+      <c r="I421" s="66"/>
       <c r="J421" s="26"/>
       <c r="K421" s="55" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="422" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B422" s="39"/>
-      <c r="C422" s="39" t="s">
+      <c r="B422" s="68"/>
+      <c r="C422" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="D422" s="39"/>
-      <c r="E422" s="39"/>
-      <c r="F422" s="39"/>
-      <c r="G422" s="39"/>
-      <c r="H422" s="39"/>
-      <c r="I422" s="39">
+      <c r="D422" s="68"/>
+      <c r="E422" s="68"/>
+      <c r="F422" s="68"/>
+      <c r="G422" s="68"/>
+      <c r="H422" s="68"/>
+      <c r="I422" s="68">
         <f>(H421)-((E423/E421*H423)+(E424/E421*H424))</f>
         <v>0.41997309402197314</v>
       </c>
@@ -32361,67 +32412,67 @@
       <c r="K422" s="55"/>
     </row>
     <row r="423" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B423" s="39"/>
-      <c r="C423" s="39"/>
-      <c r="D423" s="39" t="s">
+      <c r="B423" s="68"/>
+      <c r="C423" s="68"/>
+      <c r="D423" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="E423" s="39">
+      <c r="E423" s="68">
         <v>3</v>
       </c>
-      <c r="F423" s="39">
+      <c r="F423" s="68">
         <v>2</v>
       </c>
-      <c r="G423" s="39">
+      <c r="G423" s="68">
         <f>(E423-F423)</f>
         <v>1</v>
       </c>
-      <c r="H423" s="39">
+      <c r="H423" s="68">
         <f t="shared" ref="H423" si="135">((-F423/E423)*IMLOG2(F423/E423)+(-G423/E423)*IMLOG2(G423/E423))</f>
         <v>0.91829583405449056</v>
       </c>
-      <c r="I423" s="39"/>
+      <c r="I423" s="68"/>
       <c r="J423" s="42" t="s">
         <v>45</v>
       </c>
       <c r="K423" s="55"/>
     </row>
     <row r="424" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B424" s="39"/>
-      <c r="C424" s="39"/>
-      <c r="D424" s="39" t="s">
+      <c r="B424" s="68"/>
+      <c r="C424" s="68"/>
+      <c r="D424" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="E424" s="39">
+      <c r="E424" s="68">
         <v>2</v>
       </c>
-      <c r="F424" s="39">
-        <v>0</v>
-      </c>
-      <c r="G424" s="39">
+      <c r="F424" s="68">
+        <v>0</v>
+      </c>
+      <c r="G424" s="68">
         <f>(E424-F424)</f>
         <v>2</v>
       </c>
-      <c r="H424" s="39">
-        <v>0</v>
-      </c>
-      <c r="I424" s="39"/>
+      <c r="H424" s="68">
+        <v>0</v>
+      </c>
+      <c r="I424" s="68"/>
       <c r="J424" s="42" t="s">
         <v>26</v>
       </c>
       <c r="K424" s="55"/>
     </row>
     <row r="425" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B425" s="19"/>
-      <c r="C425" s="19" t="s">
+      <c r="B425" s="67"/>
+      <c r="C425" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="D425" s="19"/>
-      <c r="E425" s="19"/>
-      <c r="F425" s="19"/>
-      <c r="G425" s="19"/>
-      <c r="H425" s="19"/>
-      <c r="I425" s="19">
+      <c r="D425" s="67"/>
+      <c r="E425" s="67"/>
+      <c r="F425" s="67"/>
+      <c r="G425" s="67"/>
+      <c r="H425" s="67"/>
+      <c r="I425" s="67">
         <f>(H421)-((E426/E421*H426)+(E427/E421*H427)+(E428/E421*H428))</f>
         <v>0.41997309402197314</v>
       </c>
@@ -32432,86 +32483,86 @@
       <c r="K425" s="55"/>
     </row>
     <row r="426" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B426" s="19"/>
-      <c r="C426" s="19"/>
-      <c r="D426" s="19" t="s">
+      <c r="B426" s="67"/>
+      <c r="C426" s="67"/>
+      <c r="D426" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="E426" s="19">
+      <c r="E426" s="67">
         <v>3</v>
       </c>
-      <c r="F426" s="19">
+      <c r="F426" s="67">
         <v>2</v>
       </c>
-      <c r="G426" s="19">
+      <c r="G426" s="67">
         <f>E426-F426</f>
         <v>1</v>
       </c>
-      <c r="H426" s="19">
+      <c r="H426" s="67">
         <f t="shared" ref="H426" si="137">((-F426/E426)*IMLOG2(F426/E426)+(-G426/E426)*IMLOG2(G426/E426))</f>
         <v>0.91829583405449056</v>
       </c>
-      <c r="I426" s="19"/>
+      <c r="I426" s="67"/>
       <c r="J426" s="26"/>
       <c r="K426" s="55"/>
     </row>
     <row r="427" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B427" s="19"/>
-      <c r="C427" s="19"/>
-      <c r="D427" s="19" t="s">
+      <c r="B427" s="67"/>
+      <c r="C427" s="67"/>
+      <c r="D427" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="E427" s="19">
+      <c r="E427" s="67">
         <v>1</v>
       </c>
-      <c r="F427" s="19">
-        <v>0</v>
-      </c>
-      <c r="G427" s="19">
+      <c r="F427" s="67">
+        <v>0</v>
+      </c>
+      <c r="G427" s="67">
         <f t="shared" ref="G427:G428" si="138">E427-F427</f>
         <v>1</v>
       </c>
-      <c r="H427" s="19">
-        <v>0</v>
-      </c>
-      <c r="I427" s="19"/>
+      <c r="H427" s="67">
+        <v>0</v>
+      </c>
+      <c r="I427" s="67"/>
       <c r="J427" s="26"/>
       <c r="K427" s="55"/>
     </row>
     <row r="428" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B428" s="19"/>
-      <c r="C428" s="19"/>
-      <c r="D428" s="19" t="s">
+      <c r="B428" s="67"/>
+      <c r="C428" s="67"/>
+      <c r="D428" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="E428" s="19">
+      <c r="E428" s="67">
         <v>1</v>
       </c>
-      <c r="F428" s="19">
-        <v>0</v>
-      </c>
-      <c r="G428" s="19">
+      <c r="F428" s="67">
+        <v>0</v>
+      </c>
+      <c r="G428" s="67">
         <f t="shared" si="138"/>
         <v>1</v>
       </c>
-      <c r="H428" s="19">
-        <v>0</v>
-      </c>
-      <c r="I428" s="19"/>
+      <c r="H428" s="67">
+        <v>0</v>
+      </c>
+      <c r="I428" s="67"/>
       <c r="J428" s="26"/>
       <c r="K428" s="55"/>
     </row>
     <row r="429" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B429" s="19"/>
-      <c r="C429" s="19" t="s">
+      <c r="B429" s="67"/>
+      <c r="C429" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="D429" s="19"/>
-      <c r="E429" s="19"/>
-      <c r="F429" s="19"/>
-      <c r="G429" s="19"/>
-      <c r="H429" s="19"/>
-      <c r="I429" s="19">
+      <c r="D429" s="67"/>
+      <c r="E429" s="67"/>
+      <c r="F429" s="67"/>
+      <c r="G429" s="67"/>
+      <c r="H429" s="67"/>
+      <c r="I429" s="67">
         <f>(H421)-((E430/E421*H430)+(E431/E421*H431)+(E432/E421*H432))</f>
         <v>0.17095059445466743</v>
       </c>
@@ -32522,85 +32573,85 @@
       <c r="K429" s="55"/>
     </row>
     <row r="430" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B430" s="19"/>
-      <c r="C430" s="19"/>
-      <c r="D430" s="21" t="s">
+      <c r="B430" s="67"/>
+      <c r="C430" s="67"/>
+      <c r="D430" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="E430" s="19">
+      <c r="E430" s="67">
         <v>4</v>
       </c>
-      <c r="F430" s="19">
+      <c r="F430" s="67">
         <v>2</v>
       </c>
-      <c r="G430" s="19">
+      <c r="G430" s="67">
         <f t="shared" ref="G430:G431" si="140">E430-F430</f>
         <v>2</v>
       </c>
-      <c r="H430" s="19">
+      <c r="H430" s="67">
         <f>((-F430/E430)*IMLOG2(F430/E430)+(-G430/E430)*IMLOG2(G430/E430))</f>
         <v>1</v>
       </c>
-      <c r="I430" s="19"/>
+      <c r="I430" s="67"/>
       <c r="J430" s="26"/>
       <c r="K430" s="55"/>
     </row>
     <row r="431" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B431" s="19"/>
-      <c r="C431" s="19"/>
-      <c r="D431" s="21" t="s">
+      <c r="B431" s="67"/>
+      <c r="C431" s="67"/>
+      <c r="D431" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="E431" s="19">
+      <c r="E431" s="67">
         <v>1</v>
       </c>
-      <c r="F431" s="19">
-        <v>0</v>
-      </c>
-      <c r="G431" s="19">
+      <c r="F431" s="67">
+        <v>0</v>
+      </c>
+      <c r="G431" s="67">
         <f t="shared" si="140"/>
         <v>1</v>
       </c>
-      <c r="H431" s="19">
-        <v>0</v>
-      </c>
-      <c r="I431" s="19"/>
+      <c r="H431" s="67">
+        <v>0</v>
+      </c>
+      <c r="I431" s="67"/>
       <c r="J431" s="26"/>
       <c r="K431" s="55"/>
     </row>
     <row r="432" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B432" s="19"/>
-      <c r="C432" s="19"/>
-      <c r="D432" s="21" t="s">
+      <c r="B432" s="67"/>
+      <c r="C432" s="67"/>
+      <c r="D432" s="71" t="s">
         <v>169</v>
       </c>
-      <c r="E432" s="19">
-        <v>0</v>
-      </c>
-      <c r="F432" s="19">
-        <v>0</v>
-      </c>
-      <c r="G432" s="19">
-        <v>0</v>
-      </c>
-      <c r="H432" s="19">
-        <v>0</v>
-      </c>
-      <c r="I432" s="19"/>
+      <c r="E432" s="67">
+        <v>0</v>
+      </c>
+      <c r="F432" s="67">
+        <v>0</v>
+      </c>
+      <c r="G432" s="67">
+        <v>0</v>
+      </c>
+      <c r="H432" s="67">
+        <v>0</v>
+      </c>
+      <c r="I432" s="67"/>
       <c r="J432" s="26"/>
       <c r="K432" s="55"/>
     </row>
-    <row r="433" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B433" s="19"/>
-      <c r="C433" s="21" t="s">
+    <row r="433" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B433" s="67"/>
+      <c r="C433" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="D433" s="19"/>
-      <c r="E433" s="19"/>
-      <c r="F433" s="19"/>
-      <c r="G433" s="19"/>
-      <c r="H433" s="19"/>
-      <c r="I433" s="19">
+      <c r="D433" s="67"/>
+      <c r="E433" s="67"/>
+      <c r="F433" s="67"/>
+      <c r="G433" s="67"/>
+      <c r="H433" s="67"/>
+      <c r="I433" s="67">
         <f>(H421)-((E434/E421*H434)+(E435/E421*H435))</f>
         <v>0.17095059445466743</v>
       </c>
@@ -32611,63 +32662,63 @@
       <c r="K433" s="55"/>
     </row>
     <row r="434" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B434" s="19"/>
-      <c r="C434" s="19"/>
-      <c r="D434" s="21" t="s">
+      <c r="B434" s="67"/>
+      <c r="C434" s="67"/>
+      <c r="D434" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="E434" s="19">
+      <c r="E434" s="67">
         <v>1</v>
       </c>
-      <c r="F434" s="19">
-        <v>0</v>
-      </c>
-      <c r="G434" s="19">
+      <c r="F434" s="67">
+        <v>0</v>
+      </c>
+      <c r="G434" s="67">
         <f t="shared" ref="G434:G435" si="142">E434-F434</f>
         <v>1</v>
       </c>
-      <c r="H434" s="19">
-        <v>0</v>
-      </c>
-      <c r="I434" s="19"/>
+      <c r="H434" s="67">
+        <v>0</v>
+      </c>
+      <c r="I434" s="67"/>
       <c r="J434" s="26"/>
       <c r="K434" s="55"/>
     </row>
     <row r="435" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B435" s="19"/>
-      <c r="C435" s="19"/>
-      <c r="D435" s="21" t="s">
+      <c r="B435" s="67"/>
+      <c r="C435" s="67"/>
+      <c r="D435" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="E435" s="19">
+      <c r="E435" s="67">
         <v>4</v>
       </c>
-      <c r="F435" s="19">
+      <c r="F435" s="67">
         <v>2</v>
       </c>
-      <c r="G435" s="19">
+      <c r="G435" s="67">
         <f t="shared" si="142"/>
         <v>2</v>
       </c>
-      <c r="H435" s="19">
+      <c r="H435" s="67">
         <f t="shared" ref="H435" si="143">((-F435/E435)*IMLOG2(F435/E435)+(-G435/E435)*IMLOG2(G435/E435))</f>
         <v>1</v>
       </c>
-      <c r="I435" s="19"/>
+      <c r="I435" s="67"/>
       <c r="J435" s="26"/>
       <c r="K435" s="55"/>
     </row>
-    <row r="436" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B436" s="19"/>
-      <c r="C436" s="21" t="s">
+    <row r="436" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B436" s="67"/>
+      <c r="C436" s="71" t="s">
         <v>171</v>
       </c>
-      <c r="D436" s="19"/>
-      <c r="E436" s="19"/>
-      <c r="F436" s="19"/>
-      <c r="G436" s="19"/>
-      <c r="H436" s="19"/>
-      <c r="I436" s="19">
+      <c r="D436" s="67"/>
+      <c r="E436" s="67"/>
+      <c r="F436" s="67"/>
+      <c r="G436" s="67"/>
+      <c r="H436" s="67"/>
+      <c r="I436" s="67">
         <f>(H421)-((E437/E421*H437)+(E438/E421*H438)+(E439/E421*H439))</f>
         <v>0</v>
       </c>
@@ -32678,84 +32729,84 @@
       <c r="K436" s="55"/>
     </row>
     <row r="437" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B437" s="19"/>
-      <c r="C437" s="19"/>
-      <c r="D437" s="21" t="s">
+      <c r="B437" s="67"/>
+      <c r="C437" s="67"/>
+      <c r="D437" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="E437" s="19">
+      <c r="E437" s="67">
         <v>5</v>
       </c>
-      <c r="F437" s="19">
+      <c r="F437" s="67">
         <v>2</v>
       </c>
-      <c r="G437" s="19">
+      <c r="G437" s="67">
         <f t="shared" ref="G437" si="145">E437-F437</f>
         <v>3</v>
       </c>
-      <c r="H437" s="19">
+      <c r="H437" s="67">
         <f t="shared" ref="H437" si="146">((-F437/E437)*IMLOG2(F437/E437)+(-G437/E437)*IMLOG2(G437/E437))</f>
         <v>0.97095059445466747</v>
       </c>
-      <c r="I437" s="19"/>
+      <c r="I437" s="67"/>
       <c r="J437" s="26"/>
       <c r="K437" s="55"/>
     </row>
     <row r="438" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B438" s="19"/>
-      <c r="C438" s="19"/>
-      <c r="D438" s="21" t="s">
+      <c r="B438" s="67"/>
+      <c r="C438" s="67"/>
+      <c r="D438" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="E438" s="19">
-        <v>0</v>
-      </c>
-      <c r="F438" s="19">
-        <v>0</v>
-      </c>
-      <c r="G438" s="19">
-        <v>0</v>
-      </c>
-      <c r="H438" s="19">
-        <v>0</v>
-      </c>
-      <c r="I438" s="19"/>
+      <c r="E438" s="67">
+        <v>0</v>
+      </c>
+      <c r="F438" s="67">
+        <v>0</v>
+      </c>
+      <c r="G438" s="67">
+        <v>0</v>
+      </c>
+      <c r="H438" s="67">
+        <v>0</v>
+      </c>
+      <c r="I438" s="67"/>
       <c r="J438" s="26"/>
       <c r="K438" s="55"/>
     </row>
     <row r="439" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B439" s="19"/>
-      <c r="C439" s="19"/>
-      <c r="D439" s="21" t="s">
+      <c r="B439" s="67"/>
+      <c r="C439" s="67"/>
+      <c r="D439" s="71" t="s">
         <v>220</v>
       </c>
-      <c r="E439" s="19">
-        <v>0</v>
-      </c>
-      <c r="F439" s="19">
-        <v>0</v>
-      </c>
-      <c r="G439" s="19">
-        <v>0</v>
-      </c>
-      <c r="H439" s="19">
-        <v>0</v>
-      </c>
-      <c r="I439" s="19"/>
+      <c r="E439" s="67">
+        <v>0</v>
+      </c>
+      <c r="F439" s="67">
+        <v>0</v>
+      </c>
+      <c r="G439" s="67">
+        <v>0</v>
+      </c>
+      <c r="H439" s="67">
+        <v>0</v>
+      </c>
+      <c r="I439" s="67"/>
       <c r="J439" s="26"/>
       <c r="K439" s="55"/>
     </row>
-    <row r="440" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B440" s="19"/>
-      <c r="C440" s="21" t="s">
+    <row r="440" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B440" s="67"/>
+      <c r="C440" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="D440" s="19"/>
-      <c r="E440" s="19"/>
-      <c r="F440" s="19"/>
-      <c r="G440" s="19"/>
-      <c r="H440" s="19"/>
-      <c r="I440" s="19">
+      <c r="D440" s="67"/>
+      <c r="E440" s="67"/>
+      <c r="F440" s="67"/>
+      <c r="G440" s="67"/>
+      <c r="H440" s="67"/>
+      <c r="I440" s="67">
         <f>(H421)-((E441/E421*H441)+(E442/E421*H442)+(E443/E421*H443)+(E444/E421*H444))</f>
         <v>0.17095059445466743</v>
       </c>
@@ -32766,109 +32817,109 @@
       <c r="K440" s="55"/>
     </row>
     <row r="441" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B441" s="19"/>
-      <c r="C441" s="19"/>
-      <c r="D441" s="21" t="s">
+      <c r="B441" s="67"/>
+      <c r="C441" s="67"/>
+      <c r="D441" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="E441" s="19">
+      <c r="E441" s="67">
         <v>1</v>
       </c>
-      <c r="F441" s="19">
-        <v>0</v>
-      </c>
-      <c r="G441" s="19">
+      <c r="F441" s="67">
+        <v>0</v>
+      </c>
+      <c r="G441" s="67">
         <f t="shared" ref="G441:G444" si="148">E441-F441</f>
         <v>1</v>
       </c>
-      <c r="H441" s="19">
-        <v>0</v>
-      </c>
-      <c r="I441" s="19"/>
+      <c r="H441" s="67">
+        <v>0</v>
+      </c>
+      <c r="I441" s="67"/>
       <c r="J441" s="26"/>
       <c r="K441" s="55"/>
     </row>
     <row r="442" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B442" s="19"/>
-      <c r="C442" s="19"/>
-      <c r="D442" s="21" t="s">
+      <c r="B442" s="67"/>
+      <c r="C442" s="67"/>
+      <c r="D442" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="E442" s="19">
-        <v>0</v>
-      </c>
-      <c r="F442" s="19">
-        <v>0</v>
-      </c>
-      <c r="G442" s="19">
+      <c r="E442" s="67">
+        <v>0</v>
+      </c>
+      <c r="F442" s="67">
+        <v>0</v>
+      </c>
+      <c r="G442" s="67">
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
-      <c r="H442" s="19">
-        <v>0</v>
-      </c>
-      <c r="I442" s="19"/>
+      <c r="H442" s="67">
+        <v>0</v>
+      </c>
+      <c r="I442" s="67"/>
       <c r="J442" s="26"/>
       <c r="K442" s="55"/>
     </row>
     <row r="443" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B443" s="19"/>
-      <c r="C443" s="19"/>
-      <c r="D443" s="21" t="s">
+      <c r="B443" s="67"/>
+      <c r="C443" s="67"/>
+      <c r="D443" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="E443" s="19">
-        <v>0</v>
-      </c>
-      <c r="F443" s="19">
-        <v>0</v>
-      </c>
-      <c r="G443" s="19">
+      <c r="E443" s="67">
+        <v>0</v>
+      </c>
+      <c r="F443" s="67">
+        <v>0</v>
+      </c>
+      <c r="G443" s="67">
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
-      <c r="H443" s="19">
-        <v>0</v>
-      </c>
-      <c r="I443" s="19"/>
+      <c r="H443" s="67">
+        <v>0</v>
+      </c>
+      <c r="I443" s="67"/>
       <c r="J443" s="26"/>
       <c r="K443" s="55"/>
     </row>
     <row r="444" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B444" s="19"/>
-      <c r="C444" s="19"/>
-      <c r="D444" s="21" t="s">
+      <c r="B444" s="67"/>
+      <c r="C444" s="67"/>
+      <c r="D444" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="E444" s="19">
+      <c r="E444" s="67">
         <v>4</v>
       </c>
-      <c r="F444" s="19">
+      <c r="F444" s="67">
         <v>2</v>
       </c>
-      <c r="G444" s="19">
+      <c r="G444" s="67">
         <f t="shared" si="148"/>
         <v>2</v>
       </c>
-      <c r="H444" s="19">
+      <c r="H444" s="67">
         <f t="shared" ref="H444" si="149">((-F444/E444)*IMLOG2(F444/E444)+(-G444/E444)*IMLOG2(G444/E444))</f>
         <v>1</v>
       </c>
-      <c r="I444" s="19"/>
+      <c r="I444" s="67"/>
       <c r="J444" s="26"/>
       <c r="K444" s="55"/>
     </row>
-    <row r="445" spans="2:11" ht="32" x14ac:dyDescent="0.45">
-      <c r="B445" s="19"/>
-      <c r="C445" s="21" t="s">
+    <row r="445" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B445" s="67"/>
+      <c r="C445" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="D445" s="19"/>
-      <c r="E445" s="19"/>
-      <c r="F445" s="19"/>
-      <c r="G445" s="19"/>
-      <c r="H445" s="19"/>
-      <c r="I445" s="19">
+      <c r="D445" s="67"/>
+      <c r="E445" s="67"/>
+      <c r="F445" s="67"/>
+      <c r="G445" s="67"/>
+      <c r="H445" s="67"/>
+      <c r="I445" s="67">
         <f>(H421)-((E446/E421*H446)+(E447/E421*H447)+(E448/E421*H448)+(E449/E421*H449))</f>
         <v>1.9973094021973115E-2</v>
       </c>
@@ -32879,109 +32930,109 @@
       <c r="K445" s="55"/>
     </row>
     <row r="446" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B446" s="19"/>
-      <c r="C446" s="19"/>
-      <c r="D446" s="21" t="s">
+      <c r="B446" s="67"/>
+      <c r="C446" s="67"/>
+      <c r="D446" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="E446" s="19">
-        <v>0</v>
-      </c>
-      <c r="F446" s="19">
-        <v>0</v>
-      </c>
-      <c r="G446" s="19">
-        <v>0</v>
-      </c>
-      <c r="H446" s="19">
-        <v>0</v>
-      </c>
-      <c r="I446" s="19"/>
+      <c r="E446" s="67">
+        <v>0</v>
+      </c>
+      <c r="F446" s="67">
+        <v>0</v>
+      </c>
+      <c r="G446" s="67">
+        <v>0</v>
+      </c>
+      <c r="H446" s="67">
+        <v>0</v>
+      </c>
+      <c r="I446" s="67"/>
       <c r="J446" s="26"/>
       <c r="K446" s="55"/>
     </row>
     <row r="447" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B447" s="19"/>
-      <c r="C447" s="19"/>
-      <c r="D447" s="21" t="s">
+      <c r="B447" s="67"/>
+      <c r="C447" s="67"/>
+      <c r="D447" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="E447" s="19">
+      <c r="E447" s="67">
         <v>3</v>
       </c>
-      <c r="F447" s="19">
+      <c r="F447" s="67">
         <v>1</v>
       </c>
-      <c r="G447" s="19">
+      <c r="G447" s="67">
         <f t="shared" ref="G447:G449" si="151">E447-F447</f>
         <v>2</v>
       </c>
-      <c r="H447" s="19">
+      <c r="H447" s="67">
         <f t="shared" ref="H447:H448" si="152">((-F447/E447)*IMLOG2(F447/E447)+(-G447/E447)*IMLOG2(G447/E447))</f>
         <v>0.91829583405449056</v>
       </c>
-      <c r="I447" s="19"/>
+      <c r="I447" s="67"/>
       <c r="J447" s="26"/>
       <c r="K447" s="55"/>
     </row>
     <row r="448" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B448" s="19"/>
-      <c r="C448" s="19"/>
-      <c r="D448" s="21" t="s">
+      <c r="B448" s="67"/>
+      <c r="C448" s="67"/>
+      <c r="D448" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="E448" s="19">
+      <c r="E448" s="67">
         <v>2</v>
       </c>
-      <c r="F448" s="19">
+      <c r="F448" s="67">
         <v>1</v>
       </c>
-      <c r="G448" s="19">
+      <c r="G448" s="67">
         <f t="shared" si="151"/>
         <v>1</v>
       </c>
-      <c r="H448" s="19">
+      <c r="H448" s="67">
         <f t="shared" si="152"/>
         <v>1</v>
       </c>
-      <c r="I448" s="19"/>
+      <c r="I448" s="67"/>
       <c r="J448" s="26"/>
       <c r="K448" s="55"/>
     </row>
     <row r="449" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B449" s="19"/>
-      <c r="C449" s="19"/>
-      <c r="D449" s="21" t="s">
+      <c r="B449" s="67"/>
+      <c r="C449" s="67"/>
+      <c r="D449" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="E449" s="19">
+      <c r="E449" s="67">
         <v>2</v>
       </c>
-      <c r="F449" s="19">
-        <v>0</v>
-      </c>
-      <c r="G449" s="19">
+      <c r="F449" s="67">
+        <v>0</v>
+      </c>
+      <c r="G449" s="67">
         <f t="shared" si="151"/>
         <v>2</v>
       </c>
-      <c r="H449" s="19">
-        <v>0</v>
-      </c>
-      <c r="I449" s="19"/>
+      <c r="H449" s="67">
+        <v>0</v>
+      </c>
+      <c r="I449" s="67"/>
       <c r="J449" s="26"/>
       <c r="K449" s="55"/>
     </row>
     <row r="450" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B450" s="19"/>
-      <c r="C450" s="19" t="s">
+      <c r="B450" s="67"/>
+      <c r="C450" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="D450" s="19"/>
-      <c r="E450" s="19"/>
-      <c r="F450" s="19"/>
-      <c r="G450" s="19"/>
-      <c r="H450" s="19"/>
-      <c r="I450" s="19">
+      <c r="D450" s="67"/>
+      <c r="E450" s="67"/>
+      <c r="F450" s="67"/>
+      <c r="G450" s="67"/>
+      <c r="H450" s="67"/>
+      <c r="I450" s="67">
         <f>(H421)-((E451/E421*H451)+(E452/E421*H452)+(E453/E421*H453))</f>
         <v>0</v>
       </c>
@@ -32992,85 +33043,85 @@
       <c r="K450" s="55"/>
     </row>
     <row r="451" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B451" s="19"/>
-      <c r="C451" s="19"/>
-      <c r="D451" s="21" t="s">
+      <c r="B451" s="67"/>
+      <c r="C451" s="67"/>
+      <c r="D451" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="E451" s="19">
+      <c r="E451" s="67">
         <v>5</v>
       </c>
-      <c r="F451" s="19">
+      <c r="F451" s="67">
         <v>2</v>
       </c>
-      <c r="G451" s="19">
+      <c r="G451" s="67">
         <f t="shared" ref="G451" si="154">E451-F451</f>
         <v>3</v>
       </c>
-      <c r="H451" s="19">
+      <c r="H451" s="67">
         <f t="shared" ref="H451" si="155">((-F451/E451)*IMLOG2(F451/E451)+(-G451/E451)*IMLOG2(G451/E451))</f>
         <v>0.97095059445466747</v>
       </c>
-      <c r="I451" s="19"/>
+      <c r="I451" s="67"/>
       <c r="J451" s="26"/>
       <c r="K451" s="55"/>
     </row>
     <row r="452" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B452" s="19"/>
-      <c r="C452" s="19"/>
-      <c r="D452" s="21" t="s">
+      <c r="B452" s="67"/>
+      <c r="C452" s="67"/>
+      <c r="D452" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="E452" s="19">
-        <v>0</v>
-      </c>
-      <c r="F452" s="19">
-        <v>0</v>
-      </c>
-      <c r="G452" s="19">
-        <v>0</v>
-      </c>
-      <c r="H452" s="19">
-        <v>0</v>
-      </c>
-      <c r="I452" s="19"/>
+      <c r="E452" s="67">
+        <v>0</v>
+      </c>
+      <c r="F452" s="67">
+        <v>0</v>
+      </c>
+      <c r="G452" s="67">
+        <v>0</v>
+      </c>
+      <c r="H452" s="67">
+        <v>0</v>
+      </c>
+      <c r="I452" s="67"/>
       <c r="J452" s="26"/>
       <c r="K452" s="55"/>
     </row>
     <row r="453" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B453" s="19"/>
-      <c r="C453" s="19"/>
-      <c r="D453" s="21" t="s">
+      <c r="B453" s="67"/>
+      <c r="C453" s="67"/>
+      <c r="D453" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="E453" s="19">
-        <v>0</v>
-      </c>
-      <c r="F453" s="19">
-        <v>0</v>
-      </c>
-      <c r="G453" s="19">
-        <v>0</v>
-      </c>
-      <c r="H453" s="19">
-        <v>0</v>
-      </c>
-      <c r="I453" s="19"/>
+      <c r="E453" s="67">
+        <v>0</v>
+      </c>
+      <c r="F453" s="67">
+        <v>0</v>
+      </c>
+      <c r="G453" s="67">
+        <v>0</v>
+      </c>
+      <c r="H453" s="67">
+        <v>0</v>
+      </c>
+      <c r="I453" s="67"/>
       <c r="J453" s="26"/>
       <c r="K453" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K4:K54"/>
+    <mergeCell ref="K58:K104"/>
+    <mergeCell ref="K150:K196"/>
+    <mergeCell ref="K201:K242"/>
+    <mergeCell ref="K247:K288"/>
     <mergeCell ref="K293:K330"/>
     <mergeCell ref="K335:K376"/>
     <mergeCell ref="K380:K416"/>
     <mergeCell ref="K421:K453"/>
     <mergeCell ref="K108:K145"/>
-    <mergeCell ref="K4:K54"/>
-    <mergeCell ref="K58:K104"/>
-    <mergeCell ref="K150:K196"/>
-    <mergeCell ref="K201:K242"/>
-    <mergeCell ref="K247:K288"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
selesai bikin video presentasi
</commit_message>
<xml_diff>
--- a/Data Master & Uji/Data Perhitungan.xlsx
+++ b/Data Master & Uji/Data Perhitungan.xlsx
@@ -22,7 +22,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Training'!$A$1:$O$121</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22706,8 +22705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H131" sqref="H131"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29527,7 +29526,7 @@
         <v>Entropy</v>
       </c>
     </row>
-    <row r="252" spans="2:13" ht="31" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B252" s="17" t="s">
         <v>234</v>
       </c>
@@ -34869,16 +34868,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K4:K54"/>
+    <mergeCell ref="K58:K104"/>
+    <mergeCell ref="K155:K201"/>
+    <mergeCell ref="K206:K247"/>
+    <mergeCell ref="K252:K293"/>
     <mergeCell ref="K298:K335"/>
     <mergeCell ref="K340:K381"/>
     <mergeCell ref="K385:K421"/>
     <mergeCell ref="K426:K458"/>
     <mergeCell ref="K108:K150"/>
-    <mergeCell ref="K4:K54"/>
-    <mergeCell ref="K58:K104"/>
-    <mergeCell ref="K155:K201"/>
-    <mergeCell ref="K206:K247"/>
-    <mergeCell ref="K252:K293"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>